<commit_message>
Adding @Purchase @Tool and updating Database Spreadsheet
</commit_message>
<xml_diff>
--- a/Database.xlsx
+++ b/Database.xlsx
@@ -5,17 +5,19 @@
   <workbookPr autoCompressPictures="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Anthony\Dropbox\E 177\Project\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Anthony\Dropbox\E 177\GitStuff\ToolCheckGUI\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="2838" yWindow="222" windowWidth="23778" windowHeight="11082" activeTab="3"/>
+    <workbookView xWindow="2838" yWindow="222" windowWidth="23778" windowHeight="11082" activeTab="4"/>
   </bookViews>
   <sheets>
     <sheet name="Staff" sheetId="1" r:id="rId1"/>
     <sheet name="Mentor" sheetId="2" r:id="rId2"/>
     <sheet name="Student" sheetId="3" r:id="rId3"/>
     <sheet name="School" sheetId="4" r:id="rId4"/>
+    <sheet name="Purchase" sheetId="5" r:id="rId5"/>
+    <sheet name="Tools" sheetId="6" r:id="rId6"/>
   </sheets>
   <calcPr calcId="140001" concurrentCalc="0"/>
   <extLst>
@@ -30,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="8">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="16">
   <si>
     <t>Alice Chow</t>
   </si>
@@ -54,6 +56,30 @@
   </si>
   <si>
     <t>America</t>
+  </si>
+  <si>
+    <t>Sprocket</t>
+  </si>
+  <si>
+    <t>VEX Motor</t>
+  </si>
+  <si>
+    <t>VEX Brain</t>
+  </si>
+  <si>
+    <t>Angle Gusset</t>
+  </si>
+  <si>
+    <t>Clamp</t>
+  </si>
+  <si>
+    <t>Saw</t>
+  </si>
+  <si>
+    <t>Phillips Screwdriver</t>
+  </si>
+  <si>
+    <t>Punch</t>
   </si>
 </sst>
 </file>
@@ -89,8 +115,11 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -484,7 +513,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
@@ -518,4 +547,119 @@
     </ext>
   </extLst>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:C5"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C5" sqref="C5"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
+  <cols>
+    <col min="1" max="1" width="19.578125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+      <c r="A1" t="s">
+        <v>8</v>
+      </c>
+      <c r="B1">
+        <v>5</v>
+      </c>
+      <c r="C1">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+      <c r="A2" t="s">
+        <v>9</v>
+      </c>
+      <c r="B2">
+        <v>20</v>
+      </c>
+      <c r="C2">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+      <c r="A3" t="s">
+        <v>10</v>
+      </c>
+      <c r="B3">
+        <v>25</v>
+      </c>
+      <c r="C3">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+      <c r="A4" t="s">
+        <v>11</v>
+      </c>
+      <c r="B4">
+        <v>1</v>
+      </c>
+      <c r="C4">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+      <c r="C5" s="1"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:B4"/>
+  <sheetViews>
+    <sheetView topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="D24" sqref="D24"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
+  <cols>
+    <col min="1" max="1" width="15.83984375" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.55000000000000004">
+      <c r="A1" t="s">
+        <v>12</v>
+      </c>
+      <c r="B1">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.55000000000000004">
+      <c r="A2" t="s">
+        <v>13</v>
+      </c>
+      <c r="B2">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.55000000000000004">
+      <c r="A3" t="s">
+        <v>14</v>
+      </c>
+      <c r="B3">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.55000000000000004">
+      <c r="A4" t="s">
+        <v>15</v>
+      </c>
+      <c r="B4">
+        <v>5</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
udpating Database, sheet was missnamed
</commit_message>
<xml_diff>
--- a/Database.xlsx
+++ b/Database.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="2838" yWindow="222" windowWidth="23778" windowHeight="11082" activeTab="4"/>
+    <workbookView xWindow="2838" yWindow="222" windowWidth="23778" windowHeight="11082" activeTab="5"/>
   </bookViews>
   <sheets>
     <sheet name="Staff" sheetId="1" r:id="rId1"/>
@@ -17,7 +17,7 @@
     <sheet name="Student" sheetId="3" r:id="rId3"/>
     <sheet name="School" sheetId="4" r:id="rId4"/>
     <sheet name="Purchase" sheetId="5" r:id="rId5"/>
-    <sheet name="Tools" sheetId="6" r:id="rId6"/>
+    <sheet name="Tool" sheetId="6" r:id="rId6"/>
   </sheets>
   <calcPr calcId="140001" concurrentCalc="0"/>
   <extLst>
@@ -553,7 +553,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C5"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="C5" sqref="C5"/>
     </sheetView>
   </sheetViews>
@@ -618,8 +618,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B4"/>
   <sheetViews>
-    <sheetView topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="D24" sqref="D24"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D14" sqref="D14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>

</xml_diff>

<commit_message>
all Add callbacks are updated, as well as updated some back callbacks
</commit_message>
<xml_diff>
--- a/Database.xlsx
+++ b/Database.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="2838" yWindow="222" windowWidth="23778" windowHeight="11082" activeTab="2"/>
+    <workbookView xWindow="2838" yWindow="222" windowWidth="23778" windowHeight="11082" activeTab="4"/>
   </bookViews>
   <sheets>
     <sheet name="Staff" sheetId="1" r:id="rId1"/>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="18">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="31" uniqueCount="22">
   <si>
     <t>Alice Chow</t>
   </si>
@@ -86,6 +86,18 @@
   </si>
   <si>
     <t>Bishop</t>
+  </si>
+  <si>
+    <t>Jackie Ko</t>
+  </si>
+  <si>
+    <t>SFSU</t>
+  </si>
+  <si>
+    <t>Dewalt Drill</t>
+  </si>
+  <si>
+    <t>Plus Gusset</t>
   </si>
 </sst>
 </file>
@@ -406,9 +418,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:A2"/>
+  <dimension ref="A1:A3"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A3" sqref="A3"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.83984375" defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
   <cols>
@@ -425,6 +439,11 @@
         <v>7</v>
       </c>
     </row>
+    <row r="3" spans="1:1" x14ac:dyDescent="0.55000000000000004">
+      <c r="A3" t="s">
+        <v>18</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <extLst>
@@ -437,10 +456,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B2"/>
+  <dimension ref="A1:B3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C2" sqref="C2"/>
+      <selection activeCell="A3" sqref="A3:B3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.83984375" defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
@@ -465,6 +484,14 @@
         <v>5</v>
       </c>
     </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.55000000000000004">
+      <c r="A3" t="s">
+        <v>18</v>
+      </c>
+      <c r="B3" t="s">
+        <v>19</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <extLst>
@@ -477,10 +504,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B4"/>
+  <dimension ref="A1:B5"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A4" sqref="A4:B4"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A5" sqref="A5:B5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.83984375" defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
@@ -519,6 +546,14 @@
       </c>
       <c r="B4" t="s">
         <v>17</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.55000000000000004">
+      <c r="A5" t="s">
+        <v>18</v>
+      </c>
+      <c r="B5" t="s">
+        <v>19</v>
       </c>
     </row>
   </sheetData>
@@ -575,8 +610,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C5"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C5" sqref="C5"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A5" sqref="A5:C5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
@@ -629,7 +664,15 @@
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.55000000000000004">
-      <c r="C5" s="1"/>
+      <c r="A5" t="s">
+        <v>21</v>
+      </c>
+      <c r="B5">
+        <v>0.2</v>
+      </c>
+      <c r="C5" s="1">
+        <v>1000</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -638,10 +681,10 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B4"/>
+  <dimension ref="A1:B5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D14" sqref="D14"/>
+      <selection activeCell="A5" sqref="A5:B5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
@@ -681,6 +724,14 @@
         <v>5</v>
       </c>
     </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.55000000000000004">
+      <c r="A5" t="s">
+        <v>20</v>
+      </c>
+      <c r="B5">
+        <v>7</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
purchase return and buy buttons work, need to edit logs on all tool and purchase button callbacks
</commit_message>
<xml_diff>
--- a/Database.xlsx
+++ b/Database.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="2838" yWindow="222" windowWidth="23778" windowHeight="11082" activeTab="4"/>
+    <workbookView xWindow="2838" yWindow="222" windowWidth="23778" windowHeight="11082" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="Staff" sheetId="1" r:id="rId1"/>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="31" uniqueCount="22">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="23">
   <si>
     <t>Alice Chow</t>
   </si>
@@ -98,6 +98,9 @@
   </si>
   <si>
     <t>Plus Gusset</t>
+  </si>
+  <si>
+    <t>Exacto Knife</t>
   </si>
 </sst>
 </file>
@@ -570,13 +573,13 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B2"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B4" sqref="B4"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B1" sqref="B1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.83984375" defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
   <cols>
-    <col min="1" max="1" width="8.734375" customWidth="1"/>
+    <col min="1" max="1" width="11.47265625" customWidth="1"/>
     <col min="2" max="2" width="12.68359375" customWidth="1"/>
   </cols>
   <sheetData>
@@ -585,7 +588,7 @@
         <v>3</v>
       </c>
       <c r="B1">
-        <v>97.45</v>
+        <v>200</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.55000000000000004">
@@ -593,7 +596,7 @@
         <v>5</v>
       </c>
       <c r="B2">
-        <v>175</v>
+        <v>205</v>
       </c>
     </row>
   </sheetData>
@@ -610,8 +613,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C5"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A5" sqref="A5:C5"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
@@ -627,7 +630,7 @@
         <v>5</v>
       </c>
       <c r="C1">
-        <v>40</v>
+        <v>45</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.55000000000000004">
@@ -638,7 +641,7 @@
         <v>20</v>
       </c>
       <c r="C2">
-        <v>30</v>
+        <v>26</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.55000000000000004">
@@ -681,10 +684,10 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B5"/>
+  <dimension ref="A1:B6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A5" sqref="A5:B5"/>
+      <selection activeCell="A6" sqref="A6:B6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
@@ -732,6 +735,14 @@
         <v>7</v>
       </c>
     </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.55000000000000004">
+      <c r="A6" t="s">
+        <v>22</v>
+      </c>
+      <c r="B6">
+        <v>5</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
added the log table code for both Tool and Purchase Figures
</commit_message>
<xml_diff>
--- a/Database.xlsx
+++ b/Database.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="2838" yWindow="222" windowWidth="23778" windowHeight="11082" activeTab="3"/>
+    <workbookView xWindow="2838" yWindow="222" windowWidth="23778" windowHeight="11082" activeTab="5"/>
   </bookViews>
   <sheets>
     <sheet name="Staff" sheetId="1" r:id="rId1"/>
@@ -573,7 +573,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B1" sqref="B1"/>
     </sheetView>
   </sheetViews>
@@ -588,7 +588,7 @@
         <v>3</v>
       </c>
       <c r="B1">
-        <v>200</v>
+        <v>250</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.55000000000000004">
@@ -614,7 +614,7 @@
   <dimension ref="A1:C5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C2" sqref="C2"/>
+      <selection activeCell="C4" sqref="C4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
@@ -641,7 +641,7 @@
         <v>20</v>
       </c>
       <c r="C2">
-        <v>26</v>
+        <v>16</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.55000000000000004">
@@ -663,7 +663,7 @@
         <v>1</v>
       </c>
       <c r="C4">
-        <v>100</v>
+        <v>10</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.55000000000000004">
@@ -686,8 +686,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B6"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A6" sqref="A6:B6"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B1" sqref="B1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
@@ -700,7 +700,7 @@
         <v>12</v>
       </c>
       <c r="B1">
-        <v>8</v>
+        <v>0</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.55000000000000004">
@@ -732,7 +732,7 @@
         <v>20</v>
       </c>
       <c r="B5">
-        <v>7</v>
+        <v>62</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.55000000000000004">

</xml_diff>

<commit_message>
moved the GUI file from its own folder to inside the @toolCheckout folder, this is because it is only called by toolCheckout and is a method of the file
</commit_message>
<xml_diff>
--- a/Database.xlsx
+++ b/Database.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="2844" yWindow="228" windowWidth="23784" windowHeight="11088" activeTab="7"/>
+    <workbookView minimized="1" xWindow="2844" yWindow="228" windowWidth="23784" windowHeight="11088" activeTab="7"/>
   </bookViews>
   <sheets>
     <sheet name="Staff" sheetId="7" r:id="rId1"/>
@@ -3169,8 +3169,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C134"/>
   <sheetViews>
-    <sheetView topLeftCell="A128" workbookViewId="0">
-      <selection activeCell="D146" sqref="D146"/>
+    <sheetView topLeftCell="A37" workbookViewId="0">
+      <selection activeCell="A39" sqref="A39"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
@@ -4802,8 +4802,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D75"/>
   <sheetViews>
-    <sheetView topLeftCell="A26" workbookViewId="0">
-      <selection activeCell="G35" sqref="G35"/>
+    <sheetView topLeftCell="A62" workbookViewId="0">
+      <selection activeCell="A75" sqref="A75"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.89453125" defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
@@ -5954,7 +5954,7 @@
   <dimension ref="A1:D321"/>
   <sheetViews>
     <sheetView topLeftCell="A306" workbookViewId="0">
-      <selection activeCell="B316" sqref="B316"/>
+      <selection activeCell="B314" sqref="B314"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.89453125" defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
@@ -10944,8 +10944,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C56"/>
   <sheetViews>
-    <sheetView topLeftCell="A22" workbookViewId="0">
-      <selection activeCell="C37" sqref="C37"/>
+    <sheetView topLeftCell="A38" workbookViewId="0">
+      <selection activeCell="A45" sqref="A45"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
@@ -10973,7 +10973,7 @@
       </c>
       <c r="C2">
         <f t="shared" ref="C2:C36" ca="1" si="0">RANDBETWEEN(1,100)</f>
-        <v>11</v>
+        <v>6</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.55000000000000004">
@@ -10985,7 +10985,7 @@
       </c>
       <c r="C3">
         <f t="shared" ca="1" si="0"/>
-        <v>89</v>
+        <v>33</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.55000000000000004">
@@ -10997,7 +10997,7 @@
       </c>
       <c r="C4">
         <f t="shared" ca="1" si="0"/>
-        <v>89</v>
+        <v>10</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.55000000000000004">
@@ -11009,7 +11009,7 @@
       </c>
       <c r="C5">
         <f t="shared" ca="1" si="0"/>
-        <v>44</v>
+        <v>73</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.55000000000000004">
@@ -11021,7 +11021,7 @@
       </c>
       <c r="C6">
         <f t="shared" ca="1" si="0"/>
-        <v>70</v>
+        <v>11</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.55000000000000004">
@@ -11033,7 +11033,7 @@
       </c>
       <c r="C7">
         <f t="shared" ca="1" si="0"/>
-        <v>71</v>
+        <v>62</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.55000000000000004">
@@ -11045,7 +11045,7 @@
       </c>
       <c r="C8">
         <f t="shared" ca="1" si="0"/>
-        <v>63</v>
+        <v>42</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.55000000000000004">
@@ -11057,7 +11057,7 @@
       </c>
       <c r="C9">
         <f t="shared" ca="1" si="0"/>
-        <v>51</v>
+        <v>93</v>
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.55000000000000004">
@@ -11069,7 +11069,7 @@
       </c>
       <c r="C10">
         <f t="shared" ca="1" si="0"/>
-        <v>42</v>
+        <v>67</v>
       </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.55000000000000004">
@@ -11081,7 +11081,7 @@
       </c>
       <c r="C11">
         <f t="shared" ca="1" si="0"/>
-        <v>26</v>
+        <v>4</v>
       </c>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.55000000000000004">
@@ -11093,7 +11093,7 @@
       </c>
       <c r="C12">
         <f t="shared" ca="1" si="0"/>
-        <v>5</v>
+        <v>63</v>
       </c>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.55000000000000004">
@@ -11105,7 +11105,7 @@
       </c>
       <c r="C13">
         <f t="shared" ca="1" si="0"/>
-        <v>35</v>
+        <v>2</v>
       </c>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.55000000000000004">
@@ -11128,7 +11128,7 @@
       </c>
       <c r="C15">
         <f t="shared" ca="1" si="0"/>
-        <v>25</v>
+        <v>32</v>
       </c>
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.55000000000000004">
@@ -11140,7 +11140,7 @@
       </c>
       <c r="C16">
         <f t="shared" ca="1" si="0"/>
-        <v>88</v>
+        <v>94</v>
       </c>
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.55000000000000004">
@@ -11152,7 +11152,7 @@
       </c>
       <c r="C17">
         <f t="shared" ca="1" si="0"/>
-        <v>52</v>
+        <v>94</v>
       </c>
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.55000000000000004">
@@ -11164,7 +11164,7 @@
       </c>
       <c r="C18">
         <f t="shared" ca="1" si="0"/>
-        <v>64</v>
+        <v>26</v>
       </c>
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.55000000000000004">
@@ -11176,7 +11176,7 @@
       </c>
       <c r="C19">
         <f t="shared" ca="1" si="0"/>
-        <v>46</v>
+        <v>58</v>
       </c>
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.55000000000000004">
@@ -11188,7 +11188,7 @@
       </c>
       <c r="C20">
         <f t="shared" ca="1" si="0"/>
-        <v>59</v>
+        <v>30</v>
       </c>
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.55000000000000004">
@@ -11200,7 +11200,7 @@
       </c>
       <c r="C21">
         <f t="shared" ca="1" si="0"/>
-        <v>77</v>
+        <v>87</v>
       </c>
     </row>
     <row r="22" spans="1:3" x14ac:dyDescent="0.55000000000000004">
@@ -11212,7 +11212,7 @@
       </c>
       <c r="C22">
         <f t="shared" ca="1" si="0"/>
-        <v>9</v>
+        <v>37</v>
       </c>
     </row>
     <row r="23" spans="1:3" x14ac:dyDescent="0.55000000000000004">
@@ -11224,7 +11224,7 @@
       </c>
       <c r="C23">
         <f t="shared" ca="1" si="0"/>
-        <v>99</v>
+        <v>68</v>
       </c>
     </row>
     <row r="24" spans="1:3" x14ac:dyDescent="0.55000000000000004">
@@ -11236,7 +11236,7 @@
       </c>
       <c r="C24">
         <f t="shared" ca="1" si="0"/>
-        <v>62</v>
+        <v>95</v>
       </c>
     </row>
     <row r="25" spans="1:3" x14ac:dyDescent="0.55000000000000004">
@@ -11259,7 +11259,7 @@
       </c>
       <c r="C26">
         <f t="shared" ca="1" si="0"/>
-        <v>33</v>
+        <v>47</v>
       </c>
     </row>
     <row r="27" spans="1:3" x14ac:dyDescent="0.55000000000000004">
@@ -11271,7 +11271,7 @@
       </c>
       <c r="C27">
         <f t="shared" ca="1" si="0"/>
-        <v>47</v>
+        <v>43</v>
       </c>
     </row>
     <row r="28" spans="1:3" x14ac:dyDescent="0.55000000000000004">
@@ -11283,7 +11283,7 @@
       </c>
       <c r="C28">
         <f t="shared" ca="1" si="0"/>
-        <v>27</v>
+        <v>72</v>
       </c>
     </row>
     <row r="29" spans="1:3" x14ac:dyDescent="0.55000000000000004">
@@ -11318,7 +11318,7 @@
       </c>
       <c r="C31">
         <f t="shared" ca="1" si="0"/>
-        <v>4</v>
+        <v>80</v>
       </c>
     </row>
     <row r="32" spans="1:3" x14ac:dyDescent="0.55000000000000004">
@@ -11330,7 +11330,7 @@
       </c>
       <c r="C32">
         <f t="shared" ca="1" si="0"/>
-        <v>13</v>
+        <v>15</v>
       </c>
     </row>
     <row r="33" spans="1:3" x14ac:dyDescent="0.55000000000000004">
@@ -11342,7 +11342,7 @@
       </c>
       <c r="C33">
         <f t="shared" ca="1" si="0"/>
-        <v>42</v>
+        <v>39</v>
       </c>
     </row>
     <row r="34" spans="1:3" x14ac:dyDescent="0.55000000000000004">
@@ -11354,7 +11354,7 @@
       </c>
       <c r="C34">
         <f t="shared" ca="1" si="0"/>
-        <v>27</v>
+        <v>43</v>
       </c>
     </row>
     <row r="35" spans="1:3" x14ac:dyDescent="0.55000000000000004">
@@ -11366,7 +11366,7 @@
       </c>
       <c r="C35">
         <f t="shared" ca="1" si="0"/>
-        <v>47</v>
+        <v>75</v>
       </c>
     </row>
     <row r="36" spans="1:3" x14ac:dyDescent="0.55000000000000004">
@@ -11378,7 +11378,7 @@
       </c>
       <c r="C36">
         <f t="shared" ca="1" si="0"/>
-        <v>57</v>
+        <v>24</v>
       </c>
     </row>
     <row r="37" spans="1:3" x14ac:dyDescent="0.55000000000000004">
@@ -11401,7 +11401,7 @@
       </c>
       <c r="C38">
         <f t="shared" ref="C38:C56" ca="1" si="1">RANDBETWEEN(1,100)</f>
-        <v>64</v>
+        <v>84</v>
       </c>
     </row>
     <row r="39" spans="1:3" x14ac:dyDescent="0.55000000000000004">
@@ -11413,7 +11413,7 @@
       </c>
       <c r="C39">
         <f t="shared" ca="1" si="1"/>
-        <v>13</v>
+        <v>51</v>
       </c>
     </row>
     <row r="40" spans="1:3" x14ac:dyDescent="0.55000000000000004">
@@ -11425,7 +11425,7 @@
       </c>
       <c r="C40">
         <f t="shared" ca="1" si="1"/>
-        <v>88</v>
+        <v>23</v>
       </c>
     </row>
     <row r="41" spans="1:3" x14ac:dyDescent="0.55000000000000004">
@@ -11437,7 +11437,7 @@
       </c>
       <c r="C41">
         <f t="shared" ca="1" si="1"/>
-        <v>41</v>
+        <v>65</v>
       </c>
     </row>
     <row r="42" spans="1:3" x14ac:dyDescent="0.55000000000000004">
@@ -11449,7 +11449,7 @@
       </c>
       <c r="C42">
         <f t="shared" ca="1" si="1"/>
-        <v>36</v>
+        <v>38</v>
       </c>
     </row>
     <row r="43" spans="1:3" x14ac:dyDescent="0.55000000000000004">
@@ -11473,7 +11473,7 @@
       </c>
       <c r="C44">
         <f t="shared" ca="1" si="1"/>
-        <v>92</v>
+        <v>71</v>
       </c>
     </row>
     <row r="45" spans="1:3" x14ac:dyDescent="0.55000000000000004">
@@ -11485,7 +11485,7 @@
       </c>
       <c r="C45">
         <f t="shared" ca="1" si="1"/>
-        <v>86</v>
+        <v>89</v>
       </c>
     </row>
     <row r="46" spans="1:3" x14ac:dyDescent="0.55000000000000004">
@@ -11497,7 +11497,7 @@
       </c>
       <c r="C46">
         <f t="shared" ca="1" si="1"/>
-        <v>30</v>
+        <v>98</v>
       </c>
     </row>
     <row r="47" spans="1:3" x14ac:dyDescent="0.55000000000000004">
@@ -11509,7 +11509,7 @@
       </c>
       <c r="C47">
         <f t="shared" ca="1" si="1"/>
-        <v>18</v>
+        <v>61</v>
       </c>
     </row>
     <row r="48" spans="1:3" x14ac:dyDescent="0.55000000000000004">
@@ -11521,7 +11521,7 @@
       </c>
       <c r="C48">
         <f t="shared" ca="1" si="1"/>
-        <v>75</v>
+        <v>65</v>
       </c>
     </row>
     <row r="49" spans="1:3" x14ac:dyDescent="0.55000000000000004">
@@ -11533,7 +11533,7 @@
       </c>
       <c r="C49">
         <f t="shared" ca="1" si="1"/>
-        <v>95</v>
+        <v>79</v>
       </c>
     </row>
     <row r="50" spans="1:3" x14ac:dyDescent="0.55000000000000004">
@@ -11556,7 +11556,7 @@
       </c>
       <c r="C51">
         <f t="shared" ca="1" si="1"/>
-        <v>40</v>
+        <v>58</v>
       </c>
     </row>
     <row r="52" spans="1:3" x14ac:dyDescent="0.55000000000000004">
@@ -11568,7 +11568,7 @@
       </c>
       <c r="C52">
         <f t="shared" ca="1" si="1"/>
-        <v>34</v>
+        <v>10</v>
       </c>
     </row>
     <row r="53" spans="1:3" x14ac:dyDescent="0.55000000000000004">
@@ -11580,7 +11580,7 @@
       </c>
       <c r="C53">
         <f t="shared" ca="1" si="1"/>
-        <v>35</v>
+        <v>37</v>
       </c>
     </row>
     <row r="54" spans="1:3" x14ac:dyDescent="0.55000000000000004">
@@ -11592,7 +11592,7 @@
       </c>
       <c r="C54">
         <f t="shared" ca="1" si="1"/>
-        <v>66</v>
+        <v>21</v>
       </c>
     </row>
     <row r="55" spans="1:3" x14ac:dyDescent="0.55000000000000004">
@@ -11604,7 +11604,7 @@
       </c>
       <c r="C55">
         <f t="shared" ca="1" si="1"/>
-        <v>66</v>
+        <v>18</v>
       </c>
     </row>
     <row r="56" spans="1:3" x14ac:dyDescent="0.55000000000000004">
@@ -11616,7 +11616,7 @@
       </c>
       <c r="C56">
         <f t="shared" ca="1" si="1"/>
-        <v>11</v>
+        <v>1</v>
       </c>
     </row>
   </sheetData>
@@ -11629,7 +11629,7 @@
   <dimension ref="A1:B35"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B17" sqref="B17"/>
+      <selection activeCell="F10" sqref="F10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>

</xml_diff>

<commit_message>
final changes to the files. Added comments to all the files.
</commit_message>
<xml_diff>
--- a/Database.xlsx
+++ b/Database.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView minimized="1" xWindow="2844" yWindow="228" windowWidth="23784" windowHeight="11088" activeTab="7"/>
+    <workbookView xWindow="2844" yWindow="228" windowWidth="23784" windowHeight="11088" activeTab="4"/>
   </bookViews>
   <sheets>
     <sheet name="Staff" sheetId="7" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1557" uniqueCount="920">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1565" uniqueCount="927">
   <si>
     <t>Berkeley High</t>
   </si>
@@ -2794,6 +2794,27 @@
   </si>
   <si>
     <t>Charles Walston has returned 1 of VEX 393</t>
+  </si>
+  <si>
+    <t>Kevin Johnson has checked out 4 of Clamp</t>
+  </si>
+  <si>
+    <t>Kevin Johnson has returned 2 of Clamp</t>
+  </si>
+  <si>
+    <t>Kevin Johnson has purchased 5 of Limit Switch</t>
+  </si>
+  <si>
+    <t>Kevin Johnson has returned 3 of Limit Switch</t>
+  </si>
+  <si>
+    <t>Julian Patrick</t>
+  </si>
+  <si>
+    <t>Claw Hammer</t>
+  </si>
+  <si>
+    <t>VEX Controller</t>
   </si>
 </sst>
 </file>
@@ -5954,7 +5975,7 @@
   <dimension ref="A1:D321"/>
   <sheetViews>
     <sheetView topLeftCell="A306" workbookViewId="0">
-      <selection activeCell="B314" sqref="B314"/>
+      <selection activeCell="A316" sqref="A316:B316"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.89453125" defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
@@ -10690,7 +10711,12 @@
       </c>
     </row>
     <row r="316" spans="1:4" x14ac:dyDescent="0.55000000000000004">
-      <c r="B316" s="6"/>
+      <c r="A316" t="s">
+        <v>924</v>
+      </c>
+      <c r="B316" s="6" t="s">
+        <v>809</v>
+      </c>
       <c r="C316" s="6"/>
     </row>
     <row r="317" spans="1:4" x14ac:dyDescent="0.55000000000000004">
@@ -10726,7 +10752,7 @@
   <dimension ref="A1:B24"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B14" sqref="B14"/>
+      <selection activeCell="B7" sqref="B7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.89453125" defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
@@ -10788,7 +10814,7 @@
         <v>343</v>
       </c>
       <c r="B7">
-        <v>250</v>
+        <v>238</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.55000000000000004">
@@ -10942,10 +10968,10 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C56"/>
+  <dimension ref="A1:C57"/>
   <sheetViews>
-    <sheetView topLeftCell="A38" workbookViewId="0">
-      <selection activeCell="A45" sqref="A45"/>
+    <sheetView tabSelected="1" topLeftCell="A38" workbookViewId="0">
+      <selection activeCell="A57" sqref="A57:C57"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
@@ -10973,7 +10999,7 @@
       </c>
       <c r="C2">
         <f t="shared" ref="C2:C36" ca="1" si="0">RANDBETWEEN(1,100)</f>
-        <v>6</v>
+        <v>69</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.55000000000000004">
@@ -10985,7 +11011,7 @@
       </c>
       <c r="C3">
         <f t="shared" ca="1" si="0"/>
-        <v>33</v>
+        <v>44</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.55000000000000004">
@@ -10997,7 +11023,7 @@
       </c>
       <c r="C4">
         <f t="shared" ca="1" si="0"/>
-        <v>10</v>
+        <v>82</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.55000000000000004">
@@ -11009,7 +11035,7 @@
       </c>
       <c r="C5">
         <f t="shared" ca="1" si="0"/>
-        <v>73</v>
+        <v>2</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.55000000000000004">
@@ -11021,7 +11047,7 @@
       </c>
       <c r="C6">
         <f t="shared" ca="1" si="0"/>
-        <v>11</v>
+        <v>14</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.55000000000000004">
@@ -11045,7 +11071,7 @@
       </c>
       <c r="C8">
         <f t="shared" ca="1" si="0"/>
-        <v>42</v>
+        <v>95</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.55000000000000004">
@@ -11057,7 +11083,7 @@
       </c>
       <c r="C9">
         <f t="shared" ca="1" si="0"/>
-        <v>93</v>
+        <v>71</v>
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.55000000000000004">
@@ -11069,7 +11095,7 @@
       </c>
       <c r="C10">
         <f t="shared" ca="1" si="0"/>
-        <v>67</v>
+        <v>27</v>
       </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.55000000000000004">
@@ -11081,7 +11107,7 @@
       </c>
       <c r="C11">
         <f t="shared" ca="1" si="0"/>
-        <v>4</v>
+        <v>58</v>
       </c>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.55000000000000004">
@@ -11093,7 +11119,7 @@
       </c>
       <c r="C12">
         <f t="shared" ca="1" si="0"/>
-        <v>63</v>
+        <v>2</v>
       </c>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.55000000000000004">
@@ -11128,7 +11154,7 @@
       </c>
       <c r="C15">
         <f t="shared" ca="1" si="0"/>
-        <v>32</v>
+        <v>81</v>
       </c>
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.55000000000000004">
@@ -11140,7 +11166,7 @@
       </c>
       <c r="C16">
         <f t="shared" ca="1" si="0"/>
-        <v>94</v>
+        <v>36</v>
       </c>
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.55000000000000004">
@@ -11152,7 +11178,7 @@
       </c>
       <c r="C17">
         <f t="shared" ca="1" si="0"/>
-        <v>94</v>
+        <v>33</v>
       </c>
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.55000000000000004">
@@ -11164,7 +11190,7 @@
       </c>
       <c r="C18">
         <f t="shared" ca="1" si="0"/>
-        <v>26</v>
+        <v>45</v>
       </c>
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.55000000000000004">
@@ -11176,7 +11202,7 @@
       </c>
       <c r="C19">
         <f t="shared" ca="1" si="0"/>
-        <v>58</v>
+        <v>87</v>
       </c>
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.55000000000000004">
@@ -11188,7 +11214,7 @@
       </c>
       <c r="C20">
         <f t="shared" ca="1" si="0"/>
-        <v>30</v>
+        <v>100</v>
       </c>
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.55000000000000004">
@@ -11200,7 +11226,7 @@
       </c>
       <c r="C21">
         <f t="shared" ca="1" si="0"/>
-        <v>87</v>
+        <v>58</v>
       </c>
     </row>
     <row r="22" spans="1:3" x14ac:dyDescent="0.55000000000000004">
@@ -11212,7 +11238,7 @@
       </c>
       <c r="C22">
         <f t="shared" ca="1" si="0"/>
-        <v>37</v>
+        <v>51</v>
       </c>
     </row>
     <row r="23" spans="1:3" x14ac:dyDescent="0.55000000000000004">
@@ -11224,7 +11250,7 @@
       </c>
       <c r="C23">
         <f t="shared" ca="1" si="0"/>
-        <v>68</v>
+        <v>86</v>
       </c>
     </row>
     <row r="24" spans="1:3" x14ac:dyDescent="0.55000000000000004">
@@ -11236,7 +11262,7 @@
       </c>
       <c r="C24">
         <f t="shared" ca="1" si="0"/>
-        <v>95</v>
+        <v>14</v>
       </c>
     </row>
     <row r="25" spans="1:3" x14ac:dyDescent="0.55000000000000004">
@@ -11259,7 +11285,7 @@
       </c>
       <c r="C26">
         <f t="shared" ca="1" si="0"/>
-        <v>47</v>
+        <v>7</v>
       </c>
     </row>
     <row r="27" spans="1:3" x14ac:dyDescent="0.55000000000000004">
@@ -11271,7 +11297,7 @@
       </c>
       <c r="C27">
         <f t="shared" ca="1" si="0"/>
-        <v>43</v>
+        <v>91</v>
       </c>
     </row>
     <row r="28" spans="1:3" x14ac:dyDescent="0.55000000000000004">
@@ -11283,7 +11309,7 @@
       </c>
       <c r="C28">
         <f t="shared" ca="1" si="0"/>
-        <v>72</v>
+        <v>47</v>
       </c>
     </row>
     <row r="29" spans="1:3" x14ac:dyDescent="0.55000000000000004">
@@ -11295,7 +11321,7 @@
       </c>
       <c r="C29">
         <f t="shared" ca="1" si="0"/>
-        <v>26</v>
+        <v>29</v>
       </c>
     </row>
     <row r="30" spans="1:3" x14ac:dyDescent="0.55000000000000004">
@@ -11318,7 +11344,7 @@
       </c>
       <c r="C31">
         <f t="shared" ca="1" si="0"/>
-        <v>80</v>
+        <v>89</v>
       </c>
     </row>
     <row r="32" spans="1:3" x14ac:dyDescent="0.55000000000000004">
@@ -11330,7 +11356,7 @@
       </c>
       <c r="C32">
         <f t="shared" ca="1" si="0"/>
-        <v>15</v>
+        <v>56</v>
       </c>
     </row>
     <row r="33" spans="1:3" x14ac:dyDescent="0.55000000000000004">
@@ -11342,7 +11368,7 @@
       </c>
       <c r="C33">
         <f t="shared" ca="1" si="0"/>
-        <v>39</v>
+        <v>77</v>
       </c>
     </row>
     <row r="34" spans="1:3" x14ac:dyDescent="0.55000000000000004">
@@ -11354,7 +11380,7 @@
       </c>
       <c r="C34">
         <f t="shared" ca="1" si="0"/>
-        <v>43</v>
+        <v>94</v>
       </c>
     </row>
     <row r="35" spans="1:3" x14ac:dyDescent="0.55000000000000004">
@@ -11366,7 +11392,7 @@
       </c>
       <c r="C35">
         <f t="shared" ca="1" si="0"/>
-        <v>75</v>
+        <v>10</v>
       </c>
     </row>
     <row r="36" spans="1:3" x14ac:dyDescent="0.55000000000000004">
@@ -11378,7 +11404,7 @@
       </c>
       <c r="C36">
         <f t="shared" ca="1" si="0"/>
-        <v>24</v>
+        <v>49</v>
       </c>
     </row>
     <row r="37" spans="1:3" x14ac:dyDescent="0.55000000000000004">
@@ -11401,7 +11427,7 @@
       </c>
       <c r="C38">
         <f t="shared" ref="C38:C56" ca="1" si="1">RANDBETWEEN(1,100)</f>
-        <v>84</v>
+        <v>18</v>
       </c>
     </row>
     <row r="39" spans="1:3" x14ac:dyDescent="0.55000000000000004">
@@ -11413,7 +11439,7 @@
       </c>
       <c r="C39">
         <f t="shared" ca="1" si="1"/>
-        <v>51</v>
+        <v>50</v>
       </c>
     </row>
     <row r="40" spans="1:3" x14ac:dyDescent="0.55000000000000004">
@@ -11425,7 +11451,7 @@
       </c>
       <c r="C40">
         <f t="shared" ca="1" si="1"/>
-        <v>23</v>
+        <v>62</v>
       </c>
     </row>
     <row r="41" spans="1:3" x14ac:dyDescent="0.55000000000000004">
@@ -11437,7 +11463,7 @@
       </c>
       <c r="C41">
         <f t="shared" ca="1" si="1"/>
-        <v>65</v>
+        <v>2</v>
       </c>
     </row>
     <row r="42" spans="1:3" x14ac:dyDescent="0.55000000000000004">
@@ -11449,7 +11475,7 @@
       </c>
       <c r="C42">
         <f t="shared" ca="1" si="1"/>
-        <v>38</v>
+        <v>52</v>
       </c>
     </row>
     <row r="43" spans="1:3" x14ac:dyDescent="0.55000000000000004">
@@ -11461,7 +11487,7 @@
       </c>
       <c r="C43">
         <f t="shared" ca="1" si="1"/>
-        <v>27</v>
+        <v>55</v>
       </c>
     </row>
     <row r="44" spans="1:3" x14ac:dyDescent="0.55000000000000004">
@@ -11473,7 +11499,7 @@
       </c>
       <c r="C44">
         <f t="shared" ca="1" si="1"/>
-        <v>71</v>
+        <v>27</v>
       </c>
     </row>
     <row r="45" spans="1:3" x14ac:dyDescent="0.55000000000000004">
@@ -11484,8 +11510,7 @@
         <v>6</v>
       </c>
       <c r="C45">
-        <f t="shared" ca="1" si="1"/>
-        <v>89</v>
+        <v>78</v>
       </c>
     </row>
     <row r="46" spans="1:3" x14ac:dyDescent="0.55000000000000004">
@@ -11497,7 +11522,7 @@
       </c>
       <c r="C46">
         <f t="shared" ca="1" si="1"/>
-        <v>98</v>
+        <v>16</v>
       </c>
     </row>
     <row r="47" spans="1:3" x14ac:dyDescent="0.55000000000000004">
@@ -11509,7 +11534,7 @@
       </c>
       <c r="C47">
         <f t="shared" ca="1" si="1"/>
-        <v>61</v>
+        <v>48</v>
       </c>
     </row>
     <row r="48" spans="1:3" x14ac:dyDescent="0.55000000000000004">
@@ -11521,7 +11546,7 @@
       </c>
       <c r="C48">
         <f t="shared" ca="1" si="1"/>
-        <v>65</v>
+        <v>76</v>
       </c>
     </row>
     <row r="49" spans="1:3" x14ac:dyDescent="0.55000000000000004">
@@ -11533,7 +11558,7 @@
       </c>
       <c r="C49">
         <f t="shared" ca="1" si="1"/>
-        <v>79</v>
+        <v>56</v>
       </c>
     </row>
     <row r="50" spans="1:3" x14ac:dyDescent="0.55000000000000004">
@@ -11556,7 +11581,7 @@
       </c>
       <c r="C51">
         <f t="shared" ca="1" si="1"/>
-        <v>58</v>
+        <v>40</v>
       </c>
     </row>
     <row r="52" spans="1:3" x14ac:dyDescent="0.55000000000000004">
@@ -11568,7 +11593,7 @@
       </c>
       <c r="C52">
         <f t="shared" ca="1" si="1"/>
-        <v>10</v>
+        <v>73</v>
       </c>
     </row>
     <row r="53" spans="1:3" x14ac:dyDescent="0.55000000000000004">
@@ -11580,7 +11605,7 @@
       </c>
       <c r="C53">
         <f t="shared" ca="1" si="1"/>
-        <v>37</v>
+        <v>4</v>
       </c>
     </row>
     <row r="54" spans="1:3" x14ac:dyDescent="0.55000000000000004">
@@ -11592,7 +11617,7 @@
       </c>
       <c r="C54">
         <f t="shared" ca="1" si="1"/>
-        <v>21</v>
+        <v>19</v>
       </c>
     </row>
     <row r="55" spans="1:3" x14ac:dyDescent="0.55000000000000004">
@@ -11604,7 +11629,7 @@
       </c>
       <c r="C55">
         <f t="shared" ca="1" si="1"/>
-        <v>18</v>
+        <v>47</v>
       </c>
     </row>
     <row r="56" spans="1:3" x14ac:dyDescent="0.55000000000000004">
@@ -11616,7 +11641,18 @@
       </c>
       <c r="C56">
         <f t="shared" ca="1" si="1"/>
-        <v>1</v>
+        <v>84</v>
+      </c>
+    </row>
+    <row r="57" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+      <c r="A57" t="s">
+        <v>926</v>
+      </c>
+      <c r="B57">
+        <v>30</v>
+      </c>
+      <c r="C57">
+        <v>25</v>
       </c>
     </row>
   </sheetData>
@@ -11626,10 +11662,10 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B35"/>
+  <dimension ref="A1:B36"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="F10" sqref="F10"/>
+    <sheetView topLeftCell="A21" workbookViewId="0">
+      <selection activeCell="A36" sqref="A36:B36"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
@@ -11770,7 +11806,7 @@
         <v>3</v>
       </c>
       <c r="B17">
-        <v>7</v>
+        <v>5</v>
       </c>
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.55000000000000004">
@@ -11915,6 +11951,14 @@
       </c>
       <c r="B35">
         <v>1</v>
+      </c>
+    </row>
+    <row r="36" spans="1:2" x14ac:dyDescent="0.55000000000000004">
+      <c r="A36" t="s">
+        <v>925</v>
+      </c>
+      <c r="B36">
+        <v>4</v>
       </c>
     </row>
   </sheetData>
@@ -11924,10 +11968,10 @@
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B2"/>
+  <dimension ref="A1:B4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C4" sqref="C4"/>
+      <selection activeCell="A4" sqref="A4:B4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
@@ -11952,6 +11996,22 @@
         <v>42130.692731481482</v>
       </c>
     </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.55000000000000004">
+      <c r="A3" t="s">
+        <v>920</v>
+      </c>
+      <c r="B3" s="10">
+        <v>42131.733229166668</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.55000000000000004">
+      <c r="A4" t="s">
+        <v>921</v>
+      </c>
+      <c r="B4" s="10">
+        <v>42131.73400462963</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -11959,10 +12019,10 @@
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B2"/>
+  <dimension ref="A1:B4"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A5" sqref="A5"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A4" sqref="A4:B4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
@@ -11987,6 +12047,22 @@
         <v>42130.693668981483</v>
       </c>
     </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.55000000000000004">
+      <c r="A3" t="s">
+        <v>922</v>
+      </c>
+      <c r="B3" s="10">
+        <v>42131.735960648148</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.55000000000000004">
+      <c r="A4" t="s">
+        <v>923</v>
+      </c>
+      <c r="B4" s="10">
+        <v>42131.736712962964</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
fixed a stupid error with extra spaces at the end
</commit_message>
<xml_diff>
--- a/Database.xlsx
+++ b/Database.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="2844" yWindow="228" windowWidth="23784" windowHeight="11088" activeTab="1"/>
+    <workbookView xWindow="2844" yWindow="228" windowWidth="23784" windowHeight="11088" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="Staff" sheetId="7" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1565" uniqueCount="918">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1565" uniqueCount="912">
   <si>
     <t>Berkeley High</t>
   </si>
@@ -2767,24 +2767,6 @@
   </si>
   <si>
     <t>VEX Controller</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Berkeley High </t>
-  </si>
-  <si>
-    <t xml:space="preserve">Community Day </t>
-  </si>
-  <si>
-    <t xml:space="preserve">El Cerrito </t>
-  </si>
-  <si>
-    <t xml:space="preserve">Lighthouse Charter </t>
-  </si>
-  <si>
-    <t xml:space="preserve">Pinole </t>
-  </si>
-  <si>
-    <t xml:space="preserve">Ralph Bunche </t>
   </si>
   <si>
     <t>Wallenberg</t>
@@ -4796,8 +4778,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D75"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A63" workbookViewId="0">
-      <selection activeCell="B76" sqref="B76"/>
+    <sheetView topLeftCell="A62" workbookViewId="0">
+      <selection activeCell="B74" sqref="B74"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.89453125" defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
@@ -4810,7 +4792,7 @@
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A1" t="str">
-        <f>CONCATENATE(C1," ",D1)</f>
+        <f t="shared" ref="A1:A32" si="0">CONCATENATE(C1," ",D1)</f>
         <v>Carlos Sanchez</v>
       </c>
       <c r="B1" s="4" t="s">
@@ -4825,7 +4807,7 @@
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A2" t="str">
-        <f>CONCATENATE(C2," ",D2)</f>
+        <f t="shared" si="0"/>
         <v>Chase Giannini</v>
       </c>
       <c r="B2" s="4" t="s">
@@ -4840,7 +4822,7 @@
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A3" t="str">
-        <f>CONCATENATE(C3," ",D3)</f>
+        <f t="shared" si="0"/>
         <v>John Brkich</v>
       </c>
       <c r="B3" s="4" t="s">
@@ -4855,7 +4837,7 @@
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A4" t="str">
-        <f>CONCATENATE(C4," ",D4)</f>
+        <f t="shared" si="0"/>
         <v>Brian Cheng</v>
       </c>
       <c r="B4" s="4" t="s">
@@ -4870,7 +4852,7 @@
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A5" t="str">
-        <f>CONCATENATE(C5," ",D5)</f>
+        <f t="shared" si="0"/>
         <v>Juan Castillo</v>
       </c>
       <c r="B5" s="4" t="s">
@@ -4885,7 +4867,7 @@
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A6" t="str">
-        <f>CONCATENATE(C6," ",D6)</f>
+        <f t="shared" si="0"/>
         <v>Sydney McMuldroch</v>
       </c>
       <c r="B6" s="4" t="s">
@@ -4900,7 +4882,7 @@
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A7" t="str">
-        <f>CONCATENATE(C7," ",D7)</f>
+        <f t="shared" si="0"/>
         <v>Alejandro Zuniga</v>
       </c>
       <c r="B7" s="4" t="s">
@@ -4915,7 +4897,7 @@
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A8" t="str">
-        <f>CONCATENATE(C8," ",D8)</f>
+        <f t="shared" si="0"/>
         <v>Kenny Zhen</v>
       </c>
       <c r="B8" s="4" t="s">
@@ -4930,7 +4912,7 @@
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A9" t="str">
-        <f>CONCATENATE(C9," ",D9)</f>
+        <f t="shared" si="0"/>
         <v>Matthew Naranjo</v>
       </c>
       <c r="B9" s="4" t="s">
@@ -4945,7 +4927,7 @@
     </row>
     <row r="10" spans="1:4" ht="25.5" x14ac:dyDescent="0.55000000000000004">
       <c r="A10" t="str">
-        <f>CONCATENATE(C10," ",D10)</f>
+        <f t="shared" si="0"/>
         <v>Arismel Tena</v>
       </c>
       <c r="B10" s="4" t="s">
@@ -4960,7 +4942,7 @@
     </row>
     <row r="11" spans="1:4" ht="25.5" x14ac:dyDescent="0.55000000000000004">
       <c r="A11" t="str">
-        <f>CONCATENATE(C11," ",D11)</f>
+        <f t="shared" si="0"/>
         <v>Eduardo Garibay</v>
       </c>
       <c r="B11" s="4" t="s">
@@ -4975,7 +4957,7 @@
     </row>
     <row r="12" spans="1:4" ht="25.5" x14ac:dyDescent="0.55000000000000004">
       <c r="A12" t="str">
-        <f>CONCATENATE(C12," ",D12)</f>
+        <f t="shared" si="0"/>
         <v>Hermilo Ibarra-Andrade</v>
       </c>
       <c r="B12" s="4" t="s">
@@ -4990,7 +4972,7 @@
     </row>
     <row r="13" spans="1:4" ht="25.5" x14ac:dyDescent="0.55000000000000004">
       <c r="A13" t="str">
-        <f>CONCATENATE(C13," ",D13)</f>
+        <f t="shared" si="0"/>
         <v>Nicholas Entress</v>
       </c>
       <c r="B13" s="4" t="s">
@@ -5005,7 +4987,7 @@
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A14" t="str">
-        <f>CONCATENATE(C14," ",D14)</f>
+        <f t="shared" si="0"/>
         <v>Cristian Rodriguez</v>
       </c>
       <c r="B14" s="4" t="s">
@@ -5020,7 +5002,7 @@
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A15" t="str">
-        <f>CONCATENATE(C15," ",D15)</f>
+        <f t="shared" si="0"/>
         <v>Rosalba Rodriguez</v>
       </c>
       <c r="B15" s="4" t="s">
@@ -5035,11 +5017,11 @@
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A16" t="str">
-        <f>CONCATENATE(C16," ",D16)</f>
+        <f t="shared" si="0"/>
         <v>Hershal Patel</v>
       </c>
       <c r="B16" s="4" t="s">
-        <v>911</v>
+        <v>0</v>
       </c>
       <c r="C16" s="4" t="s">
         <v>187</v>
@@ -5050,11 +5032,11 @@
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A17" t="str">
-        <f>CONCATENATE(C17," ",D17)</f>
+        <f t="shared" si="0"/>
         <v>Rafayel Mkrtchyan</v>
       </c>
       <c r="B17" s="4" t="s">
-        <v>911</v>
+        <v>0</v>
       </c>
       <c r="C17" s="4" t="s">
         <v>318</v>
@@ -5065,11 +5047,11 @@
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A18" t="str">
-        <f>CONCATENATE(C18," ",D18)</f>
+        <f t="shared" si="0"/>
         <v>Tatevik Stepanyan</v>
       </c>
       <c r="B18" s="4" t="s">
-        <v>911</v>
+        <v>0</v>
       </c>
       <c r="C18" s="4" t="s">
         <v>332</v>
@@ -5080,7 +5062,7 @@
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A19" t="str">
-        <f>CONCATENATE(C19," ",D19)</f>
+        <f t="shared" si="0"/>
         <v>Andy Chu</v>
       </c>
       <c r="B19" s="4" t="s">
@@ -5095,7 +5077,7 @@
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A20" t="str">
-        <f>CONCATENATE(C20," ",D20)</f>
+        <f t="shared" si="0"/>
         <v>Anthony Bailey Jr</v>
       </c>
       <c r="B20" s="4" t="s">
@@ -5110,7 +5092,7 @@
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A21" t="str">
-        <f>CONCATENATE(C21," ",D21)</f>
+        <f t="shared" si="0"/>
         <v>Matthew Cline</v>
       </c>
       <c r="B21" s="4" t="s">
@@ -5125,11 +5107,11 @@
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A22" t="str">
-        <f>CONCATENATE(C22," ",D22)</f>
+        <f t="shared" si="0"/>
         <v>Arnold Martinez</v>
       </c>
       <c r="B22" s="4" t="s">
-        <v>912</v>
+        <v>805</v>
       </c>
       <c r="C22" s="4" t="s">
         <v>125</v>
@@ -5140,11 +5122,11 @@
     </row>
     <row r="23" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A23" t="str">
-        <f>CONCATENATE(C23," ",D23)</f>
+        <f t="shared" si="0"/>
         <v>Baladitya Yellapragada</v>
       </c>
       <c r="B23" s="4" t="s">
-        <v>912</v>
+        <v>805</v>
       </c>
       <c r="C23" s="4" t="s">
         <v>243</v>
@@ -5155,11 +5137,11 @@
     </row>
     <row r="24" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A24" t="str">
-        <f>CONCATENATE(C24," ",D24)</f>
+        <f t="shared" si="0"/>
         <v>Greta` Huang</v>
       </c>
       <c r="B24" s="4" t="s">
-        <v>912</v>
+        <v>805</v>
       </c>
       <c r="C24" s="4" t="s">
         <v>265</v>
@@ -5170,7 +5152,7 @@
     </row>
     <row r="25" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A25" t="str">
-        <f>CONCATENATE(C25," ",D25)</f>
+        <f t="shared" si="0"/>
         <v>Alexander Yu</v>
       </c>
       <c r="B25" s="4" t="s">
@@ -5185,7 +5167,7 @@
     </row>
     <row r="26" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A26" t="str">
-        <f>CONCATENATE(C26," ",D26)</f>
+        <f t="shared" si="0"/>
         <v>Kavya Madhavan</v>
       </c>
       <c r="B26" s="4" t="s">
@@ -5200,7 +5182,7 @@
     </row>
     <row r="27" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A27" t="str">
-        <f>CONCATENATE(C27," ",D27)</f>
+        <f t="shared" si="0"/>
         <v>Pinxiu Gong</v>
       </c>
       <c r="B27" s="4" t="s">
@@ -5215,11 +5197,11 @@
     </row>
     <row r="28" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A28" t="str">
-        <f>CONCATENATE(C28," ",D28)</f>
+        <f t="shared" si="0"/>
         <v>Ian McLaughlin</v>
       </c>
       <c r="B28" s="4" t="s">
-        <v>913</v>
+        <v>795</v>
       </c>
       <c r="C28" s="4" t="s">
         <v>116</v>
@@ -5230,11 +5212,11 @@
     </row>
     <row r="29" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A29" t="str">
-        <f>CONCATENATE(C29," ",D29)</f>
+        <f t="shared" si="0"/>
         <v>Samuel Heinz</v>
       </c>
       <c r="B29" s="4" t="s">
-        <v>913</v>
+        <v>795</v>
       </c>
       <c r="C29" s="4" t="s">
         <v>167</v>
@@ -5245,11 +5227,11 @@
     </row>
     <row r="30" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A30" t="str">
-        <f>CONCATENATE(C30," ",D30)</f>
+        <f t="shared" si="0"/>
         <v>William Luong</v>
       </c>
       <c r="B30" s="4" t="s">
-        <v>913</v>
+        <v>795</v>
       </c>
       <c r="C30" s="4" t="s">
         <v>173</v>
@@ -5260,7 +5242,7 @@
     </row>
     <row r="31" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A31" t="str">
-        <f>CONCATENATE(C31," ",D31)</f>
+        <f t="shared" si="0"/>
         <v>Brian Kim</v>
       </c>
       <c r="B31" s="4" t="s">
@@ -5275,7 +5257,7 @@
     </row>
     <row r="32" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A32" t="str">
-        <f>CONCATENATE(C32," ",D32)</f>
+        <f t="shared" si="0"/>
         <v>Debleena Sengupta</v>
       </c>
       <c r="B32" s="4" t="s">
@@ -5290,7 +5272,7 @@
     </row>
     <row r="33" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A33" t="str">
-        <f>CONCATENATE(C33," ",D33)</f>
+        <f t="shared" ref="A33:A64" si="1">CONCATENATE(C33," ",D33)</f>
         <v>Kyungna Kim</v>
       </c>
       <c r="B33" s="4" t="s">
@@ -5305,7 +5287,7 @@
     </row>
     <row r="34" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A34" t="str">
-        <f>CONCATENATE(C34," ",D34)</f>
+        <f t="shared" si="1"/>
         <v>Phillip Downey</v>
       </c>
       <c r="B34" s="4" t="s">
@@ -5320,7 +5302,7 @@
     </row>
     <row r="35" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A35" t="str">
-        <f>CONCATENATE(C35," ",D35)</f>
+        <f t="shared" si="1"/>
         <v>Akira Bai</v>
       </c>
       <c r="B35" s="4" t="s">
@@ -5335,7 +5317,7 @@
     </row>
     <row r="36" spans="1:4" ht="25.5" x14ac:dyDescent="0.55000000000000004">
       <c r="A36" t="str">
-        <f>CONCATENATE(C36," ",D36)</f>
+        <f t="shared" si="1"/>
         <v>Vineet Jagadeesan Nair</v>
       </c>
       <c r="B36" s="4" t="s">
@@ -5350,11 +5332,11 @@
     </row>
     <row r="37" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A37" t="str">
-        <f>CONCATENATE(C37," ",D37)</f>
+        <f t="shared" si="1"/>
         <v>Crystal Rubalcava</v>
       </c>
       <c r="B37" s="4" t="s">
-        <v>914</v>
+        <v>807</v>
       </c>
       <c r="C37" s="4" t="s">
         <v>256</v>
@@ -5365,11 +5347,11 @@
     </row>
     <row r="38" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A38" t="str">
-        <f>CONCATENATE(C38," ",D38)</f>
+        <f t="shared" si="1"/>
         <v>Lindsey Hernandez</v>
       </c>
       <c r="B38" s="4" t="s">
-        <v>914</v>
+        <v>807</v>
       </c>
       <c r="C38" s="4" t="s">
         <v>297</v>
@@ -5380,11 +5362,11 @@
     </row>
     <row r="39" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A39" t="str">
-        <f>CONCATENATE(C39," ",D39)</f>
+        <f t="shared" si="1"/>
         <v>Mandy Li</v>
       </c>
       <c r="B39" s="4" t="s">
-        <v>914</v>
+        <v>807</v>
       </c>
       <c r="C39" s="4" t="s">
         <v>8</v>
@@ -5395,11 +5377,11 @@
     </row>
     <row r="40" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A40" t="str">
-        <f>CONCATENATE(C40," ",D40)</f>
+        <f t="shared" si="1"/>
         <v>Peter Nguyen</v>
       </c>
       <c r="B40" s="4" t="s">
-        <v>914</v>
+        <v>807</v>
       </c>
       <c r="C40" s="4" t="s">
         <v>312</v>
@@ -5410,7 +5392,7 @@
     </row>
     <row r="41" spans="1:4" ht="25.5" x14ac:dyDescent="0.55000000000000004">
       <c r="A41" t="str">
-        <f>CONCATENATE(C41," ",D41)</f>
+        <f t="shared" si="1"/>
         <v>Jaime Pimentel</v>
       </c>
       <c r="B41" s="4" t="s">
@@ -5425,7 +5407,7 @@
     </row>
     <row r="42" spans="1:4" ht="25.5" x14ac:dyDescent="0.55000000000000004">
       <c r="A42" t="str">
-        <f>CONCATENATE(C42," ",D42)</f>
+        <f t="shared" si="1"/>
         <v>Kevin Durand</v>
       </c>
       <c r="B42" s="4" t="s">
@@ -5440,7 +5422,7 @@
     </row>
     <row r="43" spans="1:4" ht="25.5" x14ac:dyDescent="0.55000000000000004">
       <c r="A43" t="str">
-        <f>CONCATENATE(C43," ",D43)</f>
+        <f t="shared" si="1"/>
         <v>Wing Chuen Lam</v>
       </c>
       <c r="B43" s="4" t="s">
@@ -5455,7 +5437,7 @@
     </row>
     <row r="44" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A44" t="str">
-        <f>CONCATENATE(C44," ",D44)</f>
+        <f t="shared" si="1"/>
         <v>Kyle Archer</v>
       </c>
       <c r="B44" s="4" t="s">
@@ -5470,7 +5452,7 @@
     </row>
     <row r="45" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A45" t="str">
-        <f>CONCATENATE(C45," ",D45)</f>
+        <f t="shared" si="1"/>
         <v>Mark Tegio</v>
       </c>
       <c r="B45" s="4" t="s">
@@ -5485,7 +5467,7 @@
     </row>
     <row r="46" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A46" t="str">
-        <f>CONCATENATE(C46," ",D46)</f>
+        <f t="shared" si="1"/>
         <v>Mimi Parker</v>
       </c>
       <c r="B46" s="4" t="s">
@@ -5500,7 +5482,7 @@
     </row>
     <row r="47" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A47" t="str">
-        <f>CONCATENATE(C47," ",D47)</f>
+        <f t="shared" si="1"/>
         <v>Kevin Lee</v>
       </c>
       <c r="B47" s="4" t="s">
@@ -5515,7 +5497,7 @@
     </row>
     <row r="48" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A48" t="str">
-        <f>CONCATENATE(C48," ",D48)</f>
+        <f t="shared" si="1"/>
         <v>Rachel Ieda</v>
       </c>
       <c r="B48" s="4" t="s">
@@ -5530,7 +5512,7 @@
     </row>
     <row r="49" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A49" t="str">
-        <f>CONCATENATE(C49," ",D49)</f>
+        <f t="shared" si="1"/>
         <v>Sam Harris</v>
       </c>
       <c r="B49" s="4" t="s">
@@ -5545,7 +5527,7 @@
     </row>
     <row r="50" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A50" t="str">
-        <f>CONCATENATE(C50," ",D50)</f>
+        <f t="shared" si="1"/>
         <v>Urvashi Betarbet</v>
       </c>
       <c r="B50" s="4" t="s">
@@ -5560,7 +5542,7 @@
     </row>
     <row r="51" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A51" t="str">
-        <f>CONCATENATE(C51," ",D51)</f>
+        <f t="shared" si="1"/>
         <v>Emily Jensen</v>
       </c>
       <c r="B51" s="4" t="s">
@@ -5575,7 +5557,7 @@
     </row>
     <row r="52" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A52" t="str">
-        <f>CONCATENATE(C52," ",D52)</f>
+        <f t="shared" si="1"/>
         <v>Gurdit Chahal</v>
       </c>
       <c r="B52" s="4" t="s">
@@ -5590,7 +5572,7 @@
     </row>
     <row r="53" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A53" t="str">
-        <f>CONCATENATE(C53," ",D53)</f>
+        <f t="shared" si="1"/>
         <v>Jennifer Garcia</v>
       </c>
       <c r="B53" s="4" t="s">
@@ -5605,7 +5587,7 @@
     </row>
     <row r="54" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A54" t="str">
-        <f>CONCATENATE(C54," ",D54)</f>
+        <f t="shared" si="1"/>
         <v>Ben Sheff</v>
       </c>
       <c r="B54" s="4" t="s">
@@ -5620,7 +5602,7 @@
     </row>
     <row r="55" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A55" t="str">
-        <f>CONCATENATE(C55," ",D55)</f>
+        <f t="shared" si="1"/>
         <v>Huu Pham</v>
       </c>
       <c r="B55" s="4" t="s">
@@ -5635,7 +5617,7 @@
     </row>
     <row r="56" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A56" t="str">
-        <f>CONCATENATE(C56," ",D56)</f>
+        <f t="shared" si="1"/>
         <v>James Freret</v>
       </c>
       <c r="B56" s="4" t="s">
@@ -5650,7 +5632,7 @@
     </row>
     <row r="57" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A57" t="str">
-        <f>CONCATENATE(C57," ",D57)</f>
+        <f t="shared" si="1"/>
         <v>Charelston Chua</v>
       </c>
       <c r="B57" s="4" t="s">
@@ -5665,7 +5647,7 @@
     </row>
     <row r="58" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A58" t="str">
-        <f>CONCATENATE(C58," ",D58)</f>
+        <f t="shared" si="1"/>
         <v>Harshali Wadge</v>
       </c>
       <c r="B58" s="4" t="s">
@@ -5680,7 +5662,7 @@
     </row>
     <row r="59" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A59" t="str">
-        <f>CONCATENATE(C59," ",D59)</f>
+        <f t="shared" si="1"/>
         <v>Jesse Paterson</v>
       </c>
       <c r="B59" s="4" t="s">
@@ -5695,11 +5677,11 @@
     </row>
     <row r="60" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A60" t="str">
-        <f>CONCATENATE(C60," ",D60)</f>
+        <f t="shared" si="1"/>
         <v>Alex Liu</v>
       </c>
       <c r="B60" s="4" t="s">
-        <v>915</v>
+        <v>794</v>
       </c>
       <c r="C60" s="4" t="s">
         <v>237</v>
@@ -5710,11 +5692,11 @@
     </row>
     <row r="61" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A61" t="str">
-        <f>CONCATENATE(C61," ",D61)</f>
+        <f t="shared" si="1"/>
         <v>Christopher Wong</v>
       </c>
       <c r="B61" s="4" t="s">
-        <v>915</v>
+        <v>794</v>
       </c>
       <c r="C61" s="4" t="s">
         <v>89</v>
@@ -5725,11 +5707,11 @@
     </row>
     <row r="62" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A62" t="str">
-        <f>CONCATENATE(C62," ",D62)</f>
+        <f t="shared" si="1"/>
         <v>Micah Lyle</v>
       </c>
       <c r="B62" s="4" t="s">
-        <v>915</v>
+        <v>794</v>
       </c>
       <c r="C62" s="4" t="s">
         <v>306</v>
@@ -5740,11 +5722,11 @@
     </row>
     <row r="63" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A63" t="str">
-        <f>CONCATENATE(C63," ",D63)</f>
+        <f t="shared" si="1"/>
         <v>Dylan Dove</v>
       </c>
       <c r="B63" s="4" t="s">
-        <v>916</v>
+        <v>809</v>
       </c>
       <c r="C63" s="4" t="s">
         <v>260</v>
@@ -5755,11 +5737,11 @@
     </row>
     <row r="64" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A64" t="str">
-        <f>CONCATENATE(C64," ",D64)</f>
+        <f t="shared" si="1"/>
         <v>Ian Eigl</v>
       </c>
       <c r="B64" s="4" t="s">
-        <v>916</v>
+        <v>809</v>
       </c>
       <c r="C64" s="4" t="s">
         <v>116</v>
@@ -5770,11 +5752,11 @@
     </row>
     <row r="65" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A65" t="str">
-        <f>CONCATENATE(C65," ",D65)</f>
+        <f t="shared" ref="A65:A75" si="2">CONCATENATE(C65," ",D65)</f>
         <v>Ravneet Madaan</v>
       </c>
       <c r="B65" s="4" t="s">
-        <v>916</v>
+        <v>809</v>
       </c>
       <c r="C65" s="4" t="s">
         <v>320</v>
@@ -5785,11 +5767,11 @@
     </row>
     <row r="66" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A66" t="str">
-        <f>CONCATENATE(C66," ",D66)</f>
+        <f t="shared" si="2"/>
         <v>Saman Sabeti</v>
       </c>
       <c r="B66" s="4" t="s">
-        <v>916</v>
+        <v>809</v>
       </c>
       <c r="C66" s="4" t="s">
         <v>325</v>
@@ -5800,7 +5782,7 @@
     </row>
     <row r="67" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A67" t="str">
-        <f>CONCATENATE(C67," ",D67)</f>
+        <f t="shared" si="2"/>
         <v>Aurelia Guy</v>
       </c>
       <c r="B67" s="4" t="s">
@@ -5815,7 +5797,7 @@
     </row>
     <row r="68" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A68" t="str">
-        <f>CONCATENATE(C68," ",D68)</f>
+        <f t="shared" si="2"/>
         <v>Hurui Kifle</v>
       </c>
       <c r="B68" s="4" t="s">
@@ -5830,7 +5812,7 @@
     </row>
     <row r="69" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A69" t="str">
-        <f>CONCATENATE(C69," ",D69)</f>
+        <f t="shared" si="2"/>
         <v>Maliena Guy</v>
       </c>
       <c r="B69" s="4" t="s">
@@ -5845,7 +5827,7 @@
     </row>
     <row r="70" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A70" t="str">
-        <f>CONCATENATE(C70," ",D70)</f>
+        <f t="shared" si="2"/>
         <v>Sam Patrick</v>
       </c>
       <c r="B70" s="4" t="s">
@@ -5860,7 +5842,7 @@
     </row>
     <row r="71" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A71" t="str">
-        <f>CONCATENATE(C71," ",D71)</f>
+        <f t="shared" si="2"/>
         <v>Clancy Lee</v>
       </c>
       <c r="B71" s="4" t="s">
@@ -5875,7 +5857,7 @@
     </row>
     <row r="72" spans="1:4" ht="25.5" x14ac:dyDescent="0.55000000000000004">
       <c r="A72" t="str">
-        <f>CONCATENATE(C72," ",D72)</f>
+        <f t="shared" si="2"/>
         <v>Guangzhao (Philip) Yang</v>
       </c>
       <c r="B72" s="4" t="s">
@@ -5890,7 +5872,7 @@
     </row>
     <row r="73" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A73" t="str">
-        <f>CONCATENATE(C73," ",D73)</f>
+        <f t="shared" si="2"/>
         <v>Lucas Medino</v>
       </c>
       <c r="B73" s="4" t="s">
@@ -5905,11 +5887,11 @@
     </row>
     <row r="74" spans="1:4" ht="25.5" x14ac:dyDescent="0.55000000000000004">
       <c r="A74" t="str">
-        <f>CONCATENATE(C74," ",D74)</f>
+        <f t="shared" si="2"/>
         <v>Stephen Pereira-Schork</v>
       </c>
       <c r="B74" s="4" t="s">
-        <v>917</v>
+        <v>911</v>
       </c>
       <c r="C74" s="4" t="s">
         <v>328</v>
@@ -5920,11 +5902,11 @@
     </row>
     <row r="75" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A75" t="str">
-        <f>CONCATENATE(C75," ",D75)</f>
+        <f t="shared" si="2"/>
         <v>Terence Yang</v>
       </c>
       <c r="B75" s="4" t="s">
-        <v>917</v>
+        <v>911</v>
       </c>
       <c r="C75" s="4" t="s">
         <v>44</v>
@@ -5950,8 +5932,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D321"/>
   <sheetViews>
-    <sheetView topLeftCell="A301" workbookViewId="0">
-      <selection activeCell="B321" sqref="B321"/>
+    <sheetView topLeftCell="A298" workbookViewId="0">
+      <selection activeCell="B315" sqref="B315"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.89453125" defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
@@ -5963,7 +5945,7 @@
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A1" t="str">
-        <f>CONCATENATE(C1," ",D1)</f>
+        <f t="shared" ref="A1:A32" si="0">CONCATENATE(C1," ",D1)</f>
         <v>Kevin Lee</v>
       </c>
       <c r="B1" s="6" t="s">
@@ -5978,7 +5960,7 @@
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A2" t="str">
-        <f>CONCATENATE(C2," ",D2)</f>
+        <f t="shared" si="0"/>
         <v>Brian Lee</v>
       </c>
       <c r="B2" s="6" t="s">
@@ -5993,7 +5975,7 @@
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A3" t="str">
-        <f>CONCATENATE(C3," ",D3)</f>
+        <f t="shared" si="0"/>
         <v>Kevin Lee</v>
       </c>
       <c r="B3" s="6" t="s">
@@ -6008,7 +5990,7 @@
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A4" t="str">
-        <f>CONCATENATE(C4," ",D4)</f>
+        <f t="shared" si="0"/>
         <v>Andrew Lee</v>
       </c>
       <c r="B4" s="6" t="s">
@@ -6023,7 +6005,7 @@
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A5" t="str">
-        <f>CONCATENATE(C5," ",D5)</f>
+        <f t="shared" si="0"/>
         <v>Benjamin Lee</v>
       </c>
       <c r="B5" s="6" t="s">
@@ -6038,7 +6020,7 @@
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A6" t="str">
-        <f>CONCATENATE(C6," ",D6)</f>
+        <f t="shared" si="0"/>
         <v>Simon Lee</v>
       </c>
       <c r="B6" s="6" t="s">
@@ -6053,7 +6035,7 @@
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A7" t="str">
-        <f>CONCATENATE(C7," ",D7)</f>
+        <f t="shared" si="0"/>
         <v>Adriana Lazano</v>
       </c>
       <c r="B7" s="6" t="s">
@@ -6068,7 +6050,7 @@
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A8" t="str">
-        <f>CONCATENATE(C8," ",D8)</f>
+        <f t="shared" si="0"/>
         <v>Kevin Law</v>
       </c>
       <c r="B8" s="6" t="s">
@@ -6083,7 +6065,7 @@
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A9" t="str">
-        <f>CONCATENATE(C9," ",D9)</f>
+        <f t="shared" si="0"/>
         <v>Robert Lavryonova</v>
       </c>
       <c r="B9" s="6" t="s">
@@ -6098,7 +6080,7 @@
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A10" t="str">
-        <f>CONCATENATE(C10," ",D10)</f>
+        <f t="shared" si="0"/>
         <v>HaoYang Latt</v>
       </c>
       <c r="B10" s="6" t="s">
@@ -6113,7 +6095,7 @@
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A11" t="str">
-        <f>CONCATENATE(C11," ",D11)</f>
+        <f t="shared" si="0"/>
         <v>Levi Lara</v>
       </c>
       <c r="B11" s="6" t="s">
@@ -6128,7 +6110,7 @@
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A12" t="str">
-        <f>CONCATENATE(C12," ",D12)</f>
+        <f t="shared" si="0"/>
         <v>Johnny Lander</v>
       </c>
       <c r="B12" s="6" t="s">
@@ -6143,7 +6125,7 @@
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A13" t="str">
-        <f>CONCATENATE(C13," ",D13)</f>
+        <f t="shared" si="0"/>
         <v>Hae Landaverde</v>
       </c>
       <c r="B13" s="6" t="s">
@@ -6158,7 +6140,7 @@
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A14" t="str">
-        <f>CONCATENATE(C14," ",D14)</f>
+        <f t="shared" si="0"/>
         <v>Dylan Lam</v>
       </c>
       <c r="B14" s="6" t="s">
@@ -6173,7 +6155,7 @@
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A15" t="str">
-        <f>CONCATENATE(C15," ",D15)</f>
+        <f t="shared" si="0"/>
         <v>Kai Lakireddy</v>
       </c>
       <c r="B15" s="6" t="s">
@@ -6188,7 +6170,7 @@
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A16" t="str">
-        <f>CONCATENATE(C16," ",D16)</f>
+        <f t="shared" si="0"/>
         <v>Trayvonda Kwasriza</v>
       </c>
       <c r="B16" s="6" t="s">
@@ -6203,7 +6185,7 @@
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A17" t="str">
-        <f>CONCATENATE(C17," ",D17)</f>
+        <f t="shared" si="0"/>
         <v>Griffin Kwan</v>
       </c>
       <c r="B17" s="6" t="s">
@@ -6218,7 +6200,7 @@
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A18" t="str">
-        <f>CONCATENATE(C18," ",D18)</f>
+        <f t="shared" si="0"/>
         <v>James Kudsk</v>
       </c>
       <c r="B18" s="6" t="s">
@@ -6233,7 +6215,7 @@
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A19" t="str">
-        <f>CONCATENATE(C19," ",D19)</f>
+        <f t="shared" si="0"/>
         <v>Simon Finkelstein</v>
       </c>
       <c r="B19" s="6" t="s">
@@ -6248,7 +6230,7 @@
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A20" t="str">
-        <f>CONCATENATE(C20," ",D20)</f>
+        <f t="shared" si="0"/>
         <v>James Filoteo</v>
       </c>
       <c r="B20" s="6" t="s">
@@ -6263,7 +6245,7 @@
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A21" t="str">
-        <f>CONCATENATE(C21," ",D21)</f>
+        <f t="shared" si="0"/>
         <v>Antonio Fernandez</v>
       </c>
       <c r="B21" s="6" t="s">
@@ -6278,7 +6260,7 @@
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A22" t="str">
-        <f>CONCATENATE(C22," ",D22)</f>
+        <f t="shared" si="0"/>
         <v>James Fernandez</v>
       </c>
       <c r="B22" s="6" t="s">
@@ -6293,7 +6275,7 @@
     </row>
     <row r="23" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A23" t="str">
-        <f>CONCATENATE(C23," ",D23)</f>
+        <f t="shared" si="0"/>
         <v>Jun Feng</v>
       </c>
       <c r="B23" s="6" t="s">
@@ -6308,7 +6290,7 @@
     </row>
     <row r="24" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A24" t="str">
-        <f>CONCATENATE(C24," ",D24)</f>
+        <f t="shared" si="0"/>
         <v>Boris Feinberg</v>
       </c>
       <c r="B24" s="6" t="s">
@@ -6323,7 +6305,7 @@
     </row>
     <row r="25" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A25" t="str">
-        <f>CONCATENATE(C25," ",D25)</f>
+        <f t="shared" si="0"/>
         <v>Jose Fedorov</v>
       </c>
       <c r="B25" s="6" t="s">
@@ -6338,7 +6320,7 @@
     </row>
     <row r="26" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A26" t="str">
-        <f>CONCATENATE(C26," ",D26)</f>
+        <f t="shared" si="0"/>
         <v>Jesus Espinoza</v>
       </c>
       <c r="B26" s="6" t="s">
@@ -6353,7 +6335,7 @@
     </row>
     <row r="27" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A27" t="str">
-        <f>CONCATENATE(C27," ",D27)</f>
+        <f t="shared" si="0"/>
         <v>Wendy Espeleta</v>
       </c>
       <c r="B27" s="6" t="s">
@@ -6368,7 +6350,7 @@
     </row>
     <row r="28" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A28" t="str">
-        <f>CONCATENATE(C28," ",D28)</f>
+        <f t="shared" si="0"/>
         <v>Chenyi Escudero</v>
       </c>
       <c r="B28" s="6" t="s">
@@ -6383,7 +6365,7 @@
     </row>
     <row r="29" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A29" t="str">
-        <f>CONCATENATE(C29," ",D29)</f>
+        <f t="shared" si="0"/>
         <v>Alysha Escobar</v>
       </c>
       <c r="B29" s="6" t="s">
@@ -6398,7 +6380,7 @@
     </row>
     <row r="30" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A30" t="str">
-        <f>CONCATENATE(C30," ",D30)</f>
+        <f t="shared" si="0"/>
         <v>Carter Erdickoff</v>
       </c>
       <c r="B30" s="6" t="s">
@@ -6413,7 +6395,7 @@
     </row>
     <row r="31" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A31" t="str">
-        <f>CONCATENATE(C31," ",D31)</f>
+        <f t="shared" si="0"/>
         <v>Jarelly Embry Louden</v>
       </c>
       <c r="B31" s="6" t="s">
@@ -6428,7 +6410,7 @@
     </row>
     <row r="32" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A32" t="str">
-        <f>CONCATENATE(C32," ",D32)</f>
+        <f t="shared" si="0"/>
         <v>Austin-Jilles Eguilos</v>
       </c>
       <c r="B32" s="6" t="s">
@@ -6443,7 +6425,7 @@
     </row>
     <row r="33" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A33" t="str">
-        <f>CONCATENATE(C33," ",D33)</f>
+        <f t="shared" ref="A33:A64" si="1">CONCATENATE(C33," ",D33)</f>
         <v>Corye Duman</v>
       </c>
       <c r="B33" s="6" t="s">
@@ -6458,7 +6440,7 @@
     </row>
     <row r="34" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A34" t="str">
-        <f>CONCATENATE(C34," ",D34)</f>
+        <f t="shared" si="1"/>
         <v>Michael Driscoll</v>
       </c>
       <c r="B34" s="6" t="s">
@@ -6473,7 +6455,7 @@
     </row>
     <row r="35" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A35" t="str">
-        <f>CONCATENATE(C35," ",D35)</f>
+        <f t="shared" si="1"/>
         <v>James Drayton-Yee</v>
       </c>
       <c r="B35" s="6" t="s">
@@ -6488,7 +6470,7 @@
     </row>
     <row r="36" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A36" t="str">
-        <f>CONCATENATE(C36," ",D36)</f>
+        <f t="shared" si="1"/>
         <v>Tenzin Dong</v>
       </c>
       <c r="B36" s="6" t="s">
@@ -6503,7 +6485,7 @@
     </row>
     <row r="37" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A37" t="str">
-        <f>CONCATENATE(C37," ",D37)</f>
+        <f t="shared" si="1"/>
         <v>Christian Doi</v>
       </c>
       <c r="B37" s="6" t="s">
@@ -6518,7 +6500,7 @@
     </row>
     <row r="38" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A38" t="str">
-        <f>CONCATENATE(C38," ",D38)</f>
+        <f t="shared" si="1"/>
         <v>Alan Diaz</v>
       </c>
       <c r="B38" s="6" t="s">
@@ -6533,7 +6515,7 @@
     </row>
     <row r="39" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A39" t="str">
-        <f>CONCATENATE(C39," ",D39)</f>
+        <f t="shared" si="1"/>
         <v>Tenzin Del Toro</v>
       </c>
       <c r="B39" s="6" t="s">
@@ -6548,7 +6530,7 @@
     </row>
     <row r="40" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A40" t="str">
-        <f>CONCATENATE(C40," ",D40)</f>
+        <f t="shared" si="1"/>
         <v>Peter DaMoade</v>
       </c>
       <c r="B40" s="6" t="s">
@@ -6563,7 +6545,7 @@
     </row>
     <row r="41" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A41" t="str">
-        <f>CONCATENATE(C41," ",D41)</f>
+        <f t="shared" si="1"/>
         <v>Tazeen Cooper</v>
       </c>
       <c r="B41" s="6" t="s">
@@ -6578,7 +6560,7 @@
     </row>
     <row r="42" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A42" t="str">
-        <f>CONCATENATE(C42," ",D42)</f>
+        <f t="shared" si="1"/>
         <v>Allison Cooper</v>
       </c>
       <c r="B42" s="6" t="s">
@@ -6593,7 +6575,7 @@
     </row>
     <row r="43" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A43" t="str">
-        <f>CONCATENATE(C43," ",D43)</f>
+        <f t="shared" si="1"/>
         <v>Juan Cook</v>
       </c>
       <c r="B43" s="6" t="s">
@@ -6608,7 +6590,7 @@
     </row>
     <row r="44" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A44" t="str">
-        <f>CONCATENATE(C44," ",D44)</f>
+        <f t="shared" si="1"/>
         <v>Sandra Contreras</v>
       </c>
       <c r="B44" s="6" t="s">
@@ -6623,7 +6605,7 @@
     </row>
     <row r="45" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A45" t="str">
-        <f>CONCATENATE(C45," ",D45)</f>
+        <f t="shared" si="1"/>
         <v>Alejandro Condori</v>
       </c>
       <c r="B45" s="6" t="s">
@@ -6638,7 +6620,7 @@
     </row>
     <row r="46" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A46" t="str">
-        <f>CONCATENATE(C46," ",D46)</f>
+        <f t="shared" si="1"/>
         <v>Ehab Cisek</v>
       </c>
       <c r="B46" s="6" t="s">
@@ -6653,7 +6635,7 @@
     </row>
     <row r="47" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A47" t="str">
-        <f>CONCATENATE(C47," ",D47)</f>
+        <f t="shared" si="1"/>
         <v>Dimitri Chuck</v>
       </c>
       <c r="B47" s="6" t="s">
@@ -6668,7 +6650,7 @@
     </row>
     <row r="48" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A48" t="str">
-        <f>CONCATENATE(C48," ",D48)</f>
+        <f t="shared" si="1"/>
         <v>Tanesha Christman</v>
       </c>
       <c r="B48" s="6" t="s">
@@ -6683,7 +6665,7 @@
     </row>
     <row r="49" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A49" t="str">
-        <f>CONCATENATE(C49," ",D49)</f>
+        <f t="shared" si="1"/>
         <v>Alycia Teuscher</v>
       </c>
       <c r="B49" s="6" t="s">
@@ -6698,7 +6680,7 @@
     </row>
     <row r="50" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A50" t="str">
-        <f>CONCATENATE(C50," ",D50)</f>
+        <f t="shared" si="1"/>
         <v>Ricardo Tang</v>
       </c>
       <c r="B50" s="6" t="s">
@@ -6713,7 +6695,7 @@
     </row>
     <row r="51" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A51" t="str">
-        <f>CONCATENATE(C51," ",D51)</f>
+        <f t="shared" si="1"/>
         <v>Harrison Tan</v>
       </c>
       <c r="B51" s="6" t="s">
@@ -6728,7 +6710,7 @@
     </row>
     <row r="52" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A52" t="str">
-        <f>CONCATENATE(C52," ",D52)</f>
+        <f t="shared" si="1"/>
         <v>Gabrielle Tan</v>
       </c>
       <c r="B52" s="6" t="s">
@@ -6743,7 +6725,7 @@
     </row>
     <row r="53" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A53" t="str">
-        <f>CONCATENATE(C53," ",D53)</f>
+        <f t="shared" si="1"/>
         <v>Tiffany Tan</v>
       </c>
       <c r="B53" s="6" t="s">
@@ -6758,7 +6740,7 @@
     </row>
     <row r="54" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A54" t="str">
-        <f>CONCATENATE(C54," ",D54)</f>
+        <f t="shared" si="1"/>
         <v>Georgina Tan</v>
       </c>
       <c r="B54" s="6" t="s">
@@ -6773,7 +6755,7 @@
     </row>
     <row r="55" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A55" t="str">
-        <f>CONCATENATE(C55," ",D55)</f>
+        <f t="shared" si="1"/>
         <v>Jesus Tamayo</v>
       </c>
       <c r="B55" s="6" t="s">
@@ -6788,7 +6770,7 @@
     </row>
     <row r="56" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A56" t="str">
-        <f>CONCATENATE(C56," ",D56)</f>
+        <f t="shared" si="1"/>
         <v>William Sun</v>
       </c>
       <c r="B56" s="6" t="s">
@@ -6803,7 +6785,7 @@
     </row>
     <row r="57" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A57" t="str">
-        <f>CONCATENATE(C57," ",D57)</f>
+        <f t="shared" si="1"/>
         <v>Spencer Subrayan</v>
       </c>
       <c r="B57" s="6" t="s">
@@ -6818,7 +6800,7 @@
     </row>
     <row r="58" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A58" t="str">
-        <f>CONCATENATE(C58," ",D58)</f>
+        <f t="shared" si="1"/>
         <v>Ash Storrs</v>
       </c>
       <c r="B58" s="6" t="s">
@@ -6833,7 +6815,7 @@
     </row>
     <row r="59" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A59" t="str">
-        <f>CONCATENATE(C59," ",D59)</f>
+        <f t="shared" si="1"/>
         <v>Amy Stanfield</v>
       </c>
       <c r="B59" s="6" t="s">
@@ -6848,7 +6830,7 @@
     </row>
     <row r="60" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A60" t="str">
-        <f>CONCATENATE(C60," ",D60)</f>
+        <f t="shared" si="1"/>
         <v>Rigoberto Stacy</v>
       </c>
       <c r="B60" s="6" t="s">
@@ -6863,7 +6845,7 @@
     </row>
     <row r="61" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A61" t="str">
-        <f>CONCATENATE(C61," ",D61)</f>
+        <f t="shared" si="1"/>
         <v>Jasmine Nguyen</v>
       </c>
       <c r="B61" s="6" t="s">
@@ -6878,7 +6860,7 @@
     </row>
     <row r="62" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A62" t="str">
-        <f>CONCATENATE(C62," ",D62)</f>
+        <f t="shared" si="1"/>
         <v>Jaylin Ngo</v>
       </c>
       <c r="B62" s="6" t="s">
@@ -6893,7 +6875,7 @@
     </row>
     <row r="63" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A63" t="str">
-        <f>CONCATENATE(C63," ",D63)</f>
+        <f t="shared" si="1"/>
         <v>Fernando Ng</v>
       </c>
       <c r="B63" s="6" t="s">
@@ -6908,7 +6890,7 @@
     </row>
     <row r="64" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A64" t="str">
-        <f>CONCATENATE(C64," ",D64)</f>
+        <f t="shared" si="1"/>
         <v>Darwin Navarro</v>
       </c>
       <c r="B64" s="6" t="s">
@@ -6923,7 +6905,7 @@
     </row>
     <row r="65" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A65" t="str">
-        <f>CONCATENATE(C65," ",D65)</f>
+        <f t="shared" ref="A65:A96" si="2">CONCATENATE(C65," ",D65)</f>
         <v>Kyle Nations</v>
       </c>
       <c r="B65" s="6" t="s">
@@ -6938,7 +6920,7 @@
     </row>
     <row r="66" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A66" t="str">
-        <f>CONCATENATE(C66," ",D66)</f>
+        <f t="shared" si="2"/>
         <v>Glen Thomas Nagdev</v>
       </c>
       <c r="B66" s="6" t="s">
@@ -6953,7 +6935,7 @@
     </row>
     <row r="67" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A67" t="str">
-        <f>CONCATENATE(C67," ",D67)</f>
+        <f t="shared" si="2"/>
         <v>Oscar Munoz</v>
       </c>
       <c r="B67" s="6" t="s">
@@ -6968,7 +6950,7 @@
     </row>
     <row r="68" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A68" t="str">
-        <f>CONCATENATE(C68," ",D68)</f>
+        <f t="shared" si="2"/>
         <v>Jennifer Mueller</v>
       </c>
       <c r="B68" s="6" t="s">
@@ -6983,7 +6965,7 @@
     </row>
     <row r="69" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A69" t="str">
-        <f>CONCATENATE(C69," ",D69)</f>
+        <f t="shared" si="2"/>
         <v>Lauren Mubachir</v>
       </c>
       <c r="B69" s="6" t="s">
@@ -6998,7 +6980,7 @@
     </row>
     <row r="70" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A70" t="str">
-        <f>CONCATENATE(C70," ",D70)</f>
+        <f t="shared" si="2"/>
         <v>Gustavo Moya</v>
       </c>
       <c r="B70" s="6" t="s">
@@ -7013,7 +6995,7 @@
     </row>
     <row r="71" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A71" t="str">
-        <f>CONCATENATE(C71," ",D71)</f>
+        <f t="shared" si="2"/>
         <v>Henry Morton</v>
       </c>
       <c r="B71" s="6" t="s">
@@ -7028,7 +7010,7 @@
     </row>
     <row r="72" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A72" t="str">
-        <f>CONCATENATE(C72," ",D72)</f>
+        <f t="shared" si="2"/>
         <v>Jocelyn Bao</v>
       </c>
       <c r="B72" s="6" t="s">
@@ -7043,7 +7025,7 @@
     </row>
     <row r="73" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A73" t="str">
-        <f>CONCATENATE(C73," ",D73)</f>
+        <f t="shared" si="2"/>
         <v>Hannalei Banevicius</v>
       </c>
       <c r="B73" s="6" t="s">
@@ -7058,7 +7040,7 @@
     </row>
     <row r="74" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A74" t="str">
-        <f>CONCATENATE(C74," ",D74)</f>
+        <f t="shared" si="2"/>
         <v>Eduardo Balonos</v>
       </c>
       <c r="B74" s="6" t="s">
@@ -7073,7 +7055,7 @@
     </row>
     <row r="75" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A75" t="str">
-        <f>CONCATENATE(C75," ",D75)</f>
+        <f t="shared" si="2"/>
         <v>Hank Badalyan</v>
       </c>
       <c r="B75" s="6" t="s">
@@ -7088,7 +7070,7 @@
     </row>
     <row r="76" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A76" t="str">
-        <f>CONCATENATE(C76," ",D76)</f>
+        <f t="shared" si="2"/>
         <v>Weicheng Baba</v>
       </c>
       <c r="B76" s="6" t="s">
@@ -7103,7 +7085,7 @@
     </row>
     <row r="77" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A77" t="str">
-        <f>CONCATENATE(C77," ",D77)</f>
+        <f t="shared" si="2"/>
         <v>Thomas Avelar-Lopez</v>
       </c>
       <c r="B77" s="6" t="s">
@@ -7118,7 +7100,7 @@
     </row>
     <row r="78" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A78" t="str">
-        <f>CONCATENATE(C78," ",D78)</f>
+        <f t="shared" si="2"/>
         <v>Jonathan Ashraf</v>
       </c>
       <c r="B78" s="6" t="s">
@@ -7133,7 +7115,7 @@
     </row>
     <row r="79" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A79" t="str">
-        <f>CONCATENATE(C79," ",D79)</f>
+        <f t="shared" si="2"/>
         <v>Jessica Arciga</v>
       </c>
       <c r="B79" s="6" t="s">
@@ -7148,7 +7130,7 @@
     </row>
     <row r="80" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A80" t="str">
-        <f>CONCATENATE(C80," ",D80)</f>
+        <f t="shared" si="2"/>
         <v>Deliliah Alonso</v>
       </c>
       <c r="B80" s="6" t="s">
@@ -7163,7 +7145,7 @@
     </row>
     <row r="81" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A81" t="str">
-        <f>CONCATENATE(C81," ",D81)</f>
+        <f t="shared" si="2"/>
         <v>Cesar Alcala</v>
       </c>
       <c r="B81" s="6" t="s">
@@ -7178,7 +7160,7 @@
     </row>
     <row r="82" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A82" t="str">
-        <f>CONCATENATE(C82," ",D82)</f>
+        <f t="shared" si="2"/>
         <v>Vera Aguilar</v>
       </c>
       <c r="B82" s="6" t="s">
@@ -7193,7 +7175,7 @@
     </row>
     <row r="83" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A83" t="str">
-        <f>CONCATENATE(C83," ",D83)</f>
+        <f t="shared" si="2"/>
         <v>Carlos Aguayo</v>
       </c>
       <c r="B83" s="6" t="s">
@@ -7208,7 +7190,7 @@
     </row>
     <row r="84" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A84" t="str">
-        <f>CONCATENATE(C84," ",D84)</f>
+        <f t="shared" si="2"/>
         <v>Anson Jiang</v>
       </c>
       <c r="B84" s="6" t="s">
@@ -7223,7 +7205,7 @@
     </row>
     <row r="85" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A85" t="str">
-        <f>CONCATENATE(C85," ",D85)</f>
+        <f t="shared" si="2"/>
         <v>Claudia Jian</v>
       </c>
       <c r="B85" s="6" t="s">
@@ -7238,7 +7220,7 @@
     </row>
     <row r="86" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A86" t="str">
-        <f>CONCATENATE(C86," ",D86)</f>
+        <f t="shared" si="2"/>
         <v>Justice Jackson</v>
       </c>
       <c r="B86" s="6" t="s">
@@ -7253,7 +7235,7 @@
     </row>
     <row r="87" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A87" t="str">
-        <f>CONCATENATE(C87," ",D87)</f>
+        <f t="shared" si="2"/>
         <v>Simon Iliralium</v>
       </c>
       <c r="B87" s="6" t="s">
@@ -7268,7 +7250,7 @@
     </row>
     <row r="88" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A88" t="str">
-        <f>CONCATENATE(C88," ",D88)</f>
+        <f t="shared" si="2"/>
         <v>Jackie Ibarra</v>
       </c>
       <c r="B88" s="6" t="s">
@@ -7283,7 +7265,7 @@
     </row>
     <row r="89" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A89" t="str">
-        <f>CONCATENATE(C89," ",D89)</f>
+        <f t="shared" si="2"/>
         <v>Jaime Hurt</v>
       </c>
       <c r="B89" s="6" t="s">
@@ -7298,7 +7280,7 @@
     </row>
     <row r="90" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A90" t="str">
-        <f>CONCATENATE(C90," ",D90)</f>
+        <f t="shared" si="2"/>
         <v>Joshua Hurley</v>
       </c>
       <c r="B90" s="6" t="s">
@@ -7313,7 +7295,7 @@
     </row>
     <row r="91" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A91" t="str">
-        <f>CONCATENATE(C91," ",D91)</f>
+        <f t="shared" si="2"/>
         <v>Adrian Hunter</v>
       </c>
       <c r="B91" s="6" t="s">
@@ -7328,7 +7310,7 @@
     </row>
     <row r="92" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A92" t="str">
-        <f>CONCATENATE(C92," ",D92)</f>
+        <f t="shared" si="2"/>
         <v>Deon Hunt</v>
       </c>
       <c r="B92" s="6" t="s">
@@ -7343,7 +7325,7 @@
     </row>
     <row r="93" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A93" t="str">
-        <f>CONCATENATE(C93," ",D93)</f>
+        <f t="shared" si="2"/>
         <v>Ayanna Hubahib</v>
       </c>
       <c r="B93" s="6" t="s">
@@ -7358,7 +7340,7 @@
     </row>
     <row r="94" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A94" t="str">
-        <f>CONCATENATE(C94," ",D94)</f>
+        <f t="shared" si="2"/>
         <v>Gabriel Huang</v>
       </c>
       <c r="B94" s="6" t="s">
@@ -7373,7 +7355,7 @@
     </row>
     <row r="95" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A95" t="str">
-        <f>CONCATENATE(C95," ",D95)</f>
+        <f t="shared" si="2"/>
         <v>Hector Hu</v>
       </c>
       <c r="B95" s="6" t="s">
@@ -7388,7 +7370,7 @@
     </row>
     <row r="96" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A96" t="str">
-        <f>CONCATENATE(C96," ",D96)</f>
+        <f t="shared" si="2"/>
         <v>Victor Hsu</v>
       </c>
       <c r="B96" s="6" t="s">
@@ -7403,7 +7385,7 @@
     </row>
     <row r="97" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A97" t="str">
-        <f>CONCATENATE(C97," ",D97)</f>
+        <f t="shared" ref="A97:A128" si="3">CONCATENATE(C97," ",D97)</f>
         <v>Opal Hilario</v>
       </c>
       <c r="B97" s="6" t="s">
@@ -7418,7 +7400,7 @@
     </row>
     <row r="98" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A98" t="str">
-        <f>CONCATENATE(C98," ",D98)</f>
+        <f t="shared" si="3"/>
         <v>Erika Herrera-Ross</v>
       </c>
       <c r="B98" s="6" t="s">
@@ -7433,7 +7415,7 @@
     </row>
     <row r="99" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A99" t="str">
-        <f>CONCATENATE(C99," ",D99)</f>
+        <f t="shared" si="3"/>
         <v>Johnny Hernandez</v>
       </c>
       <c r="B99" s="6" t="s">
@@ -7448,7 +7430,7 @@
     </row>
     <row r="100" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A100" t="str">
-        <f>CONCATENATE(C100," ",D100)</f>
+        <f t="shared" si="3"/>
         <v>Abby Hernandez</v>
       </c>
       <c r="B100" s="6" t="s">
@@ -7463,7 +7445,7 @@
     </row>
     <row r="101" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A101" t="str">
-        <f>CONCATENATE(C101," ",D101)</f>
+        <f t="shared" si="3"/>
         <v>Thomas Hernandez</v>
       </c>
       <c r="B101" s="6" t="s">
@@ -7478,7 +7460,7 @@
     </row>
     <row r="102" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A102" t="str">
-        <f>CONCATENATE(C102," ",D102)</f>
+        <f t="shared" si="3"/>
         <v>Anna Henthorn-Iwane</v>
       </c>
       <c r="B102" s="6" t="s">
@@ -7493,7 +7475,7 @@
     </row>
     <row r="103" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A103" t="str">
-        <f>CONCATENATE(C103," ",D103)</f>
+        <f t="shared" si="3"/>
         <v>Billy Henderson</v>
       </c>
       <c r="B103" s="6" t="s">
@@ -7508,7 +7490,7 @@
     </row>
     <row r="104" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A104" t="str">
-        <f>CONCATENATE(C104," ",D104)</f>
+        <f t="shared" si="3"/>
         <v>Nicholas Heard</v>
       </c>
       <c r="B104" s="6" t="s">
@@ -7523,7 +7505,7 @@
     </row>
     <row r="105" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A105" t="str">
-        <f>CONCATENATE(C105," ",D105)</f>
+        <f t="shared" si="3"/>
         <v>Zoe Kidder</v>
       </c>
       <c r="B105" s="6" t="s">
@@ -7538,7 +7520,7 @@
     </row>
     <row r="106" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A106" t="str">
-        <f>CONCATENATE(C106," ",D106)</f>
+        <f t="shared" si="3"/>
         <v>Julian Khadka</v>
       </c>
       <c r="B106" s="6" t="s">
@@ -7553,7 +7535,7 @@
     </row>
     <row r="107" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A107" t="str">
-        <f>CONCATENATE(C107," ",D107)</f>
+        <f t="shared" si="3"/>
         <v>Evan Keohan</v>
       </c>
       <c r="B107" s="6" t="s">
@@ -7568,7 +7550,7 @@
     </row>
     <row r="108" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A108" t="str">
-        <f>CONCATENATE(C108," ",D108)</f>
+        <f t="shared" si="3"/>
         <v>Michelle Kelly</v>
       </c>
       <c r="B108" s="6" t="s">
@@ -7583,7 +7565,7 @@
     </row>
     <row r="109" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A109" t="str">
-        <f>CONCATENATE(C109," ",D109)</f>
+        <f t="shared" si="3"/>
         <v>Jasper Kebade</v>
       </c>
       <c r="B109" s="6" t="s">
@@ -7598,7 +7580,7 @@
     </row>
     <row r="110" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A110" t="str">
-        <f>CONCATENATE(C110," ",D110)</f>
+        <f t="shared" si="3"/>
         <v>Emilio Karnik</v>
       </c>
       <c r="B110" s="6" t="s">
@@ -7613,7 +7595,7 @@
     </row>
     <row r="111" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A111" t="str">
-        <f>CONCATENATE(C111," ",D111)</f>
+        <f t="shared" si="3"/>
         <v>Cody Jue</v>
       </c>
       <c r="B111" s="6" t="s">
@@ -7628,7 +7610,7 @@
     </row>
     <row r="112" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A112" t="str">
-        <f>CONCATENATE(C112," ",D112)</f>
+        <f t="shared" si="3"/>
         <v>Vivian Johnstone</v>
       </c>
       <c r="B112" s="6" t="s">
@@ -7643,7 +7625,7 @@
     </row>
     <row r="113" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A113" t="str">
-        <f>CONCATENATE(C113," ",D113)</f>
+        <f t="shared" si="3"/>
         <v>Kevin Johnson</v>
       </c>
       <c r="B113" s="6" t="s">
@@ -7658,7 +7640,7 @@
     </row>
     <row r="114" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A114" t="str">
-        <f>CONCATENATE(C114," ",D114)</f>
+        <f t="shared" si="3"/>
         <v>Galmandahk Jimenez</v>
       </c>
       <c r="B114" s="6" t="s">
@@ -7673,7 +7655,7 @@
     </row>
     <row r="115" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A115" t="str">
-        <f>CONCATENATE(C115," ",D115)</f>
+        <f t="shared" si="3"/>
         <v>Nick Jimenez</v>
       </c>
       <c r="B115" s="6" t="s">
@@ -7688,7 +7670,7 @@
     </row>
     <row r="116" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A116" t="str">
-        <f>CONCATENATE(C116," ",D116)</f>
+        <f t="shared" si="3"/>
         <v>Branden Chow</v>
       </c>
       <c r="B116" s="6" t="s">
@@ -7703,7 +7685,7 @@
     </row>
     <row r="117" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A117" t="str">
-        <f>CONCATENATE(C117," ",D117)</f>
+        <f t="shared" si="3"/>
         <v>Charlie Cherry</v>
       </c>
       <c r="B117" s="6" t="s">
@@ -7718,7 +7700,7 @@
     </row>
     <row r="118" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A118" t="str">
-        <f>CONCATENATE(C118," ",D118)</f>
+        <f t="shared" si="3"/>
         <v>Wilbur Cherg</v>
       </c>
       <c r="B118" s="6" t="s">
@@ -7733,7 +7715,7 @@
     </row>
     <row r="119" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A119" t="str">
-        <f>CONCATENATE(C119," ",D119)</f>
+        <f t="shared" si="3"/>
         <v>Peter Chen</v>
       </c>
       <c r="B119" s="6" t="s">
@@ -7748,7 +7730,7 @@
     </row>
     <row r="120" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A120" t="str">
-        <f>CONCATENATE(C120," ",D120)</f>
+        <f t="shared" si="3"/>
         <v>Scott Chen</v>
       </c>
       <c r="B120" s="6" t="s">
@@ -7763,7 +7745,7 @@
     </row>
     <row r="121" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A121" t="str">
-        <f>CONCATENATE(C121," ",D121)</f>
+        <f t="shared" si="3"/>
         <v>Ana Caton</v>
       </c>
       <c r="B121" s="6" t="s">
@@ -7778,7 +7760,7 @@
     </row>
     <row r="122" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A122" t="str">
-        <f>CONCATENATE(C122," ",D122)</f>
+        <f t="shared" si="3"/>
         <v>Andy (Jian Ting) He</v>
       </c>
       <c r="B122" s="6" t="s">
@@ -7793,7 +7775,7 @@
     </row>
     <row r="123" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A123" t="str">
-        <f>CONCATENATE(C123," ",D123)</f>
+        <f t="shared" si="3"/>
         <v>Justin He</v>
       </c>
       <c r="B123" s="6" t="s">
@@ -7808,7 +7790,7 @@
     </row>
     <row r="124" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A124" t="str">
-        <f>CONCATENATE(C124," ",D124)</f>
+        <f t="shared" si="3"/>
         <v>Irina Haruyama</v>
       </c>
       <c r="B124" s="6" t="s">
@@ -7823,7 +7805,7 @@
     </row>
     <row r="125" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A125" t="str">
-        <f>CONCATENATE(C125," ",D125)</f>
+        <f t="shared" si="3"/>
         <v>Madelynn Harper</v>
       </c>
       <c r="B125" s="6" t="s">
@@ -7838,7 +7820,7 @@
     </row>
     <row r="126" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A126" t="str">
-        <f>CONCATENATE(C126," ",D126)</f>
+        <f t="shared" si="3"/>
         <v>Cheryll Guitvan</v>
       </c>
       <c r="B126" s="6" t="s">
@@ -7853,7 +7835,7 @@
     </row>
     <row r="127" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A127" t="str">
-        <f>CONCATENATE(C127," ",D127)</f>
+        <f t="shared" si="3"/>
         <v>Oscar Gonzalez-Perez</v>
       </c>
       <c r="B127" s="6" t="s">
@@ -7868,7 +7850,7 @@
     </row>
     <row r="128" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A128" t="str">
-        <f>CONCATENATE(C128," ",D128)</f>
+        <f t="shared" si="3"/>
         <v>Angelina Gonzalez</v>
       </c>
       <c r="B128" s="6" t="s">
@@ -7883,7 +7865,7 @@
     </row>
     <row r="129" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A129" t="str">
-        <f>CONCATENATE(C129," ",D129)</f>
+        <f t="shared" ref="A129:A160" si="4">CONCATENATE(C129," ",D129)</f>
         <v>Mohammad Gonzalez</v>
       </c>
       <c r="B129" s="6" t="s">
@@ -7898,7 +7880,7 @@
     </row>
     <row r="130" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A130" t="str">
-        <f>CONCATENATE(C130," ",D130)</f>
+        <f t="shared" si="4"/>
         <v>Alexander Gomez</v>
       </c>
       <c r="B130" s="6" t="s">
@@ -7913,7 +7895,7 @@
     </row>
     <row r="131" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A131" t="str">
-        <f>CONCATENATE(C131," ",D131)</f>
+        <f t="shared" si="4"/>
         <v>Jeremy Gomez</v>
       </c>
       <c r="B131" s="6" t="s">
@@ -7928,7 +7910,7 @@
     </row>
     <row r="132" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A132" t="str">
-        <f>CONCATENATE(C132," ",D132)</f>
+        <f t="shared" si="4"/>
         <v>Seif Goess</v>
       </c>
       <c r="B132" s="6" t="s">
@@ -7943,7 +7925,7 @@
     </row>
     <row r="133" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A133" t="str">
-        <f>CONCATENATE(C133," ",D133)</f>
+        <f t="shared" si="4"/>
         <v>Giovanni Ghiglieri</v>
       </c>
       <c r="B133" s="6" t="s">
@@ -7958,7 +7940,7 @@
     </row>
     <row r="134" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A134" t="str">
-        <f>CONCATENATE(C134," ",D134)</f>
+        <f t="shared" si="4"/>
         <v>Enzo Gellman</v>
       </c>
       <c r="B134" s="6" t="s">
@@ -7973,7 +7955,7 @@
     </row>
     <row r="135" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A135" t="str">
-        <f>CONCATENATE(C135," ",D135)</f>
+        <f t="shared" si="4"/>
         <v>Jason Gardner</v>
       </c>
       <c r="B135" s="6" t="s">
@@ -7988,7 +7970,7 @@
     </row>
     <row r="136" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A136" t="str">
-        <f>CONCATENATE(C136," ",D136)</f>
+        <f t="shared" si="4"/>
         <v>Jorge Galeana</v>
       </c>
       <c r="B136" s="6" t="s">
@@ -8003,7 +7985,7 @@
     </row>
     <row r="137" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A137" t="str">
-        <f>CONCATENATE(C137," ",D137)</f>
+        <f t="shared" si="4"/>
         <v>Griffin Gaim</v>
       </c>
       <c r="B137" s="6" t="s">
@@ -8018,7 +8000,7 @@
     </row>
     <row r="138" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A138" t="str">
-        <f>CONCATENATE(C138," ",D138)</f>
+        <f t="shared" si="4"/>
         <v>Carter Fong</v>
       </c>
       <c r="B138" s="6" t="s">
@@ -8033,7 +8015,7 @@
     </row>
     <row r="139" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A139" t="str">
-        <f>CONCATENATE(C139," ",D139)</f>
+        <f t="shared" si="4"/>
         <v>Giovanni Sanchez</v>
       </c>
       <c r="B139" s="6" t="s">
@@ -8048,7 +8030,7 @@
     </row>
     <row r="140" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A140" t="str">
-        <f>CONCATENATE(C140," ",D140)</f>
+        <f t="shared" si="4"/>
         <v>Adan Sanchez</v>
       </c>
       <c r="B140" s="6" t="s">
@@ -8063,7 +8045,7 @@
     </row>
     <row r="141" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A141" t="str">
-        <f>CONCATENATE(C141," ",D141)</f>
+        <f t="shared" si="4"/>
         <v>Brissa Ruiz</v>
       </c>
       <c r="B141" s="6" t="s">
@@ -8078,7 +8060,7 @@
     </row>
     <row r="142" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A142" t="str">
-        <f>CONCATENATE(C142," ",D142)</f>
+        <f t="shared" si="4"/>
         <v>Reginae Rue</v>
       </c>
       <c r="B142" s="6" t="s">
@@ -8093,7 +8075,7 @@
     </row>
     <row r="143" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A143" t="str">
-        <f>CONCATENATE(C143," ",D143)</f>
+        <f t="shared" si="4"/>
         <v>Brandon Rubi</v>
       </c>
       <c r="B143" s="6" t="s">
@@ -8108,7 +8090,7 @@
     </row>
     <row r="144" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A144" t="str">
-        <f>CONCATENATE(C144," ",D144)</f>
+        <f t="shared" si="4"/>
         <v>Stephanie Rose</v>
       </c>
       <c r="B144" s="6" t="s">
@@ -8123,7 +8105,7 @@
     </row>
     <row r="145" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A145" t="str">
-        <f>CONCATENATE(C145," ",D145)</f>
+        <f t="shared" si="4"/>
         <v>Robert Rosales</v>
       </c>
       <c r="B145" s="6" t="s">
@@ -8138,7 +8120,7 @@
     </row>
     <row r="146" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A146" t="str">
-        <f>CONCATENATE(C146," ",D146)</f>
+        <f t="shared" si="4"/>
         <v>Maria Rodriguez Silva</v>
       </c>
       <c r="B146" s="6" t="s">
@@ -8153,7 +8135,7 @@
     </row>
     <row r="147" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A147" t="str">
-        <f>CONCATENATE(C147," ",D147)</f>
+        <f t="shared" si="4"/>
         <v>Julia Robertson</v>
       </c>
       <c r="B147" s="6" t="s">
@@ -8168,7 +8150,7 @@
     </row>
     <row r="148" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A148" t="str">
-        <f>CONCATENATE(C148," ",D148)</f>
+        <f t="shared" si="4"/>
         <v>Paul Robbins</v>
       </c>
       <c r="B148" s="6" t="s">
@@ -8183,7 +8165,7 @@
     </row>
     <row r="149" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A149" t="str">
-        <f>CONCATENATE(C149," ",D149)</f>
+        <f t="shared" si="4"/>
         <v>Manuel Riley</v>
       </c>
       <c r="B149" s="6" t="s">
@@ -8198,7 +8180,7 @@
     </row>
     <row r="150" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A150" t="str">
-        <f>CONCATENATE(C150," ",D150)</f>
+        <f t="shared" si="4"/>
         <v>Austin Reed</v>
       </c>
       <c r="B150" s="6" t="s">
@@ -8213,7 +8195,7 @@
     </row>
     <row r="151" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A151" t="str">
-        <f>CONCATENATE(C151," ",D151)</f>
+        <f t="shared" si="4"/>
         <v>Reginald Ranman</v>
       </c>
       <c r="B151" s="6" t="s">
@@ -8228,7 +8210,7 @@
     </row>
     <row r="152" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A152" t="str">
-        <f>CONCATENATE(C152," ",D152)</f>
+        <f t="shared" si="4"/>
         <v>Jose Ramos</v>
       </c>
       <c r="B152" s="9" t="s">
@@ -8243,7 +8225,7 @@
     </row>
     <row r="153" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A153" t="str">
-        <f>CONCATENATE(C153," ",D153)</f>
+        <f t="shared" si="4"/>
         <v>Bryan Yang</v>
       </c>
       <c r="B153" s="6" t="s">
@@ -8258,7 +8240,7 @@
     </row>
     <row r="154" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A154" t="str">
-        <f>CONCATENATE(C154," ",D154)</f>
+        <f t="shared" si="4"/>
         <v>Vytautas Xu</v>
       </c>
       <c r="B154" s="6" t="s">
@@ -8273,7 +8255,7 @@
     </row>
     <row r="155" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A155" t="str">
-        <f>CONCATENATE(C155," ",D155)</f>
+        <f t="shared" si="4"/>
         <v>Luka Xie</v>
       </c>
       <c r="B155" s="6" t="s">
@@ -8288,7 +8270,7 @@
     </row>
     <row r="156" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A156" t="str">
-        <f>CONCATENATE(C156," ",D156)</f>
+        <f t="shared" si="4"/>
         <v>Maite Wu</v>
       </c>
       <c r="B156" s="6" t="s">
@@ -8303,7 +8285,7 @@
     </row>
     <row r="157" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A157" t="str">
-        <f>CONCATENATE(C157," ",D157)</f>
+        <f t="shared" si="4"/>
         <v>Lena Wu</v>
       </c>
       <c r="B157" s="6" t="s">
@@ -8318,7 +8300,7 @@
     </row>
     <row r="158" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A158" t="str">
-        <f>CONCATENATE(C158," ",D158)</f>
+        <f t="shared" si="4"/>
         <v>Henry Wu</v>
       </c>
       <c r="B158" s="6" t="s">
@@ -8333,7 +8315,7 @@
     </row>
     <row r="159" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A159" t="str">
-        <f>CONCATENATE(C159," ",D159)</f>
+        <f t="shared" si="4"/>
         <v>Sara Woods</v>
       </c>
       <c r="B159" s="6" t="s">
@@ -8348,7 +8330,7 @@
     </row>
     <row r="160" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A160" t="str">
-        <f>CONCATENATE(C160," ",D160)</f>
+        <f t="shared" si="4"/>
         <v>Michaelangelo Wood</v>
       </c>
       <c r="B160" s="6" t="s">
@@ -8363,7 +8345,7 @@
     </row>
     <row r="161" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A161" t="str">
-        <f>CONCATENATE(C161," ",D161)</f>
+        <f t="shared" ref="A161:A168" si="5">CONCATENATE(C161," ",D161)</f>
         <v>Andrea Wong</v>
       </c>
       <c r="B161" s="6" t="s">
@@ -8378,7 +8360,7 @@
     </row>
     <row r="162" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A162" t="str">
-        <f>CONCATENATE(C162," ",D162)</f>
+        <f t="shared" si="5"/>
         <v>Elias Wong</v>
       </c>
       <c r="B162" s="6" t="s">
@@ -8393,7 +8375,7 @@
     </row>
     <row r="163" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A163" t="str">
-        <f>CONCATENATE(C163," ",D163)</f>
+        <f t="shared" si="5"/>
         <v>Michael Wong</v>
       </c>
       <c r="B163" s="6" t="s">
@@ -8408,7 +8390,7 @@
     </row>
     <row r="164" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A164" t="str">
-        <f>CONCATENATE(C164," ",D164)</f>
+        <f t="shared" si="5"/>
         <v>Elson Wong</v>
       </c>
       <c r="B164" s="6" t="s">
@@ -8423,7 +8405,7 @@
     </row>
     <row r="165" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A165" t="str">
-        <f>CONCATENATE(C165," ",D165)</f>
+        <f t="shared" si="5"/>
         <v>Jake Wisherop</v>
       </c>
       <c r="B165" s="6" t="s">
@@ -8438,7 +8420,7 @@
     </row>
     <row r="166" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A166" t="str">
-        <f>CONCATENATE(C166," ",D166)</f>
+        <f t="shared" si="5"/>
         <v>Michaelangelo Wilson</v>
       </c>
       <c r="B166" s="6" t="s">
@@ -8453,7 +8435,7 @@
     </row>
     <row r="167" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A167" t="str">
-        <f>CONCATENATE(C167," ",D167)</f>
+        <f t="shared" si="5"/>
         <v>Camilia Williams</v>
       </c>
       <c r="B167" s="6" t="s">
@@ -8468,7 +8450,7 @@
     </row>
     <row r="168" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A168" t="str">
-        <f>CONCATENATE(C168," ",D168)</f>
+        <f t="shared" si="5"/>
         <v>Philip White</v>
       </c>
       <c r="B168" s="6" t="s">
@@ -8492,7 +8474,7 @@
     </row>
     <row r="170" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A170" t="str">
-        <f>CONCATENATE(C170," ",D170)</f>
+        <f t="shared" ref="A170:A201" si="6">CONCATENATE(C170," ",D170)</f>
         <v>John Carlos Yang</v>
       </c>
       <c r="B170" s="6" t="s">
@@ -8507,7 +8489,7 @@
     </row>
     <row r="171" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A171" t="str">
-        <f>CONCATENATE(C171," ",D171)</f>
+        <f t="shared" si="6"/>
         <v>Emily Castellanos</v>
       </c>
       <c r="B171" s="6" t="s">
@@ -8522,7 +8504,7 @@
     </row>
     <row r="172" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A172" t="str">
-        <f>CONCATENATE(C172," ",D172)</f>
+        <f t="shared" si="6"/>
         <v>Joshu Carrillo</v>
       </c>
       <c r="B172" s="6" t="s">
@@ -8537,7 +8519,7 @@
     </row>
     <row r="173" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A173" t="str">
-        <f>CONCATENATE(C173," ",D173)</f>
+        <f t="shared" si="6"/>
         <v>Jasmine Calva</v>
       </c>
       <c r="B173" s="6" t="s">
@@ -8552,7 +8534,7 @@
     </row>
     <row r="174" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A174" t="str">
-        <f>CONCATENATE(C174," ",D174)</f>
+        <f t="shared" si="6"/>
         <v>Allen Cacho</v>
       </c>
       <c r="B174" s="6" t="s">
@@ -8567,7 +8549,7 @@
     </row>
     <row r="175" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A175" t="str">
-        <f>CONCATENATE(C175," ",D175)</f>
+        <f t="shared" si="6"/>
         <v>Taylor Burns</v>
       </c>
       <c r="B175" s="6" t="s">
@@ -8582,7 +8564,7 @@
     </row>
     <row r="176" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A176" t="str">
-        <f>CONCATENATE(C176," ",D176)</f>
+        <f t="shared" si="6"/>
         <v>Pedro Budker</v>
       </c>
       <c r="B176" s="6" t="s">
@@ -8597,7 +8579,7 @@
     </row>
     <row r="177" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A177" t="str">
-        <f>CONCATENATE(C177," ",D177)</f>
+        <f t="shared" si="6"/>
         <v>James Bruce</v>
       </c>
       <c r="B177" s="6" t="s">
@@ -8612,7 +8594,7 @@
     </row>
     <row r="178" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A178" t="str">
-        <f>CONCATENATE(C178," ",D178)</f>
+        <f t="shared" si="6"/>
         <v>Bryce Brown</v>
       </c>
       <c r="B178" s="6" t="s">
@@ -8627,7 +8609,7 @@
     </row>
     <row r="179" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A179" t="str">
-        <f>CONCATENATE(C179," ",D179)</f>
+        <f t="shared" si="6"/>
         <v>Jennifer Bonilla</v>
       </c>
       <c r="B179" s="6" t="s">
@@ -8642,7 +8624,7 @@
     </row>
     <row r="180" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A180" t="str">
-        <f>CONCATENATE(C180," ",D180)</f>
+        <f t="shared" si="6"/>
         <v>Kobe Bolanos</v>
       </c>
       <c r="B180" s="6" t="s">
@@ -8657,7 +8639,7 @@
     </row>
     <row r="181" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A181" t="str">
-        <f>CONCATENATE(C181," ",D181)</f>
+        <f t="shared" si="6"/>
         <v>Chris Blendstrup</v>
       </c>
       <c r="B181" s="6" t="s">
@@ -8672,7 +8654,7 @@
     </row>
     <row r="182" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A182" t="str">
-        <f>CONCATENATE(C182," ",D182)</f>
+        <f t="shared" si="6"/>
         <v>Karina Bishop</v>
       </c>
       <c r="B182" s="6" t="s">
@@ -8687,7 +8669,7 @@
     </row>
     <row r="183" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A183" t="str">
-        <f>CONCATENATE(C183," ",D183)</f>
+        <f t="shared" si="6"/>
         <v>Reejan Beverly</v>
       </c>
       <c r="B183" s="6" t="s">
@@ -8702,7 +8684,7 @@
     </row>
     <row r="184" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A184" t="str">
-        <f>CONCATENATE(C184," ",D184)</f>
+        <f t="shared" si="6"/>
         <v>Alan Becerra</v>
       </c>
       <c r="B184" s="6" t="s">
@@ -8717,7 +8699,7 @@
     </row>
     <row r="185" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A185" t="str">
-        <f>CONCATENATE(C185," ",D185)</f>
+        <f t="shared" si="6"/>
         <v>Huiyun Battas</v>
       </c>
       <c r="B185" s="6" t="s">
@@ -8732,7 +8714,7 @@
     </row>
     <row r="186" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A186" t="str">
-        <f>CONCATENATE(C186," ",D186)</f>
+        <f t="shared" si="6"/>
         <v>Noah Bassak</v>
       </c>
       <c r="B186" s="6" t="s">
@@ -8747,7 +8729,7 @@
     </row>
     <row r="187" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A187" t="str">
-        <f>CONCATENATE(C187," ",D187)</f>
+        <f t="shared" si="6"/>
         <v>Ian Bartlett</v>
       </c>
       <c r="B187" s="6" t="s">
@@ -8762,7 +8744,7 @@
     </row>
     <row r="188" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A188" t="str">
-        <f>CONCATENATE(C188," ",D188)</f>
+        <f t="shared" si="6"/>
         <v>Andrew Wenzler</v>
       </c>
       <c r="B188" s="6" t="s">
@@ -8777,7 +8759,7 @@
     </row>
     <row r="189" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A189" t="str">
-        <f>CONCATENATE(C189," ",D189)</f>
+        <f t="shared" si="6"/>
         <v>Conor Wang</v>
       </c>
       <c r="B189" s="6" t="s">
@@ -8792,7 +8774,7 @@
     </row>
     <row r="190" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A190" t="str">
-        <f>CONCATENATE(C190," ",D190)</f>
+        <f t="shared" si="6"/>
         <v>Jesse Wang</v>
       </c>
       <c r="B190" s="6" t="s">
@@ -8807,7 +8789,7 @@
     </row>
     <row r="191" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A191" t="str">
-        <f>CONCATENATE(C191," ",D191)</f>
+        <f t="shared" si="6"/>
         <v>Maggie Wan</v>
       </c>
       <c r="B191" s="6" t="s">
@@ -8822,7 +8804,7 @@
     </row>
     <row r="192" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A192" t="str">
-        <f>CONCATENATE(C192," ",D192)</f>
+        <f t="shared" si="6"/>
         <v>Charles Walston</v>
       </c>
       <c r="B192" s="6" t="s">
@@ -8837,7 +8819,7 @@
     </row>
     <row r="193" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A193" t="str">
-        <f>CONCATENATE(C193," ",D193)</f>
+        <f t="shared" si="6"/>
         <v>Roisin Wai</v>
       </c>
       <c r="B193" s="6" t="s">
@@ -8852,7 +8834,7 @@
     </row>
     <row r="194" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A194" t="str">
-        <f>CONCATENATE(C194," ",D194)</f>
+        <f t="shared" si="6"/>
         <v>Marisa Vojvoda</v>
       </c>
       <c r="B194" s="6" t="s">
@@ -8867,7 +8849,7 @@
     </row>
     <row r="195" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A195" t="str">
-        <f>CONCATENATE(C195," ",D195)</f>
+        <f t="shared" si="6"/>
         <v>Nicholas VanHeuit</v>
       </c>
       <c r="B195" s="6" t="s">
@@ -8882,7 +8864,7 @@
     </row>
     <row r="196" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A196" t="str">
-        <f>CONCATENATE(C196," ",D196)</f>
+        <f t="shared" si="6"/>
         <v>Aubrey-rose Valva</v>
       </c>
       <c r="B196" s="6" t="s">
@@ -8897,7 +8879,7 @@
     </row>
     <row r="197" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A197" t="str">
-        <f>CONCATENATE(C197," ",D197)</f>
+        <f t="shared" si="6"/>
         <v>William Valdivia</v>
       </c>
       <c r="B197" s="6" t="s">
@@ -8912,7 +8894,7 @@
     </row>
     <row r="198" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A198" t="str">
-        <f>CONCATENATE(C198," ",D198)</f>
+        <f t="shared" si="6"/>
         <v>Ethan Unurbaatar</v>
       </c>
       <c r="B198" s="6" t="s">
@@ -8927,7 +8909,7 @@
     </row>
     <row r="199" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A199" t="str">
-        <f>CONCATENATE(C199," ",D199)</f>
+        <f t="shared" si="6"/>
         <v>Jenny Tse</v>
       </c>
       <c r="B199" s="6" t="s">
@@ -8942,7 +8924,7 @@
     </row>
     <row r="200" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A200" t="str">
-        <f>CONCATENATE(C200," ",D200)</f>
+        <f t="shared" si="6"/>
         <v>Elana Truong</v>
       </c>
       <c r="B200" s="6" t="s">
@@ -8957,7 +8939,7 @@
     </row>
     <row r="201" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A201" t="str">
-        <f>CONCATENATE(C201," ",D201)</f>
+        <f t="shared" si="6"/>
         <v>Jeff Triadi</v>
       </c>
       <c r="B201" s="6" t="s">
@@ -8972,7 +8954,7 @@
     </row>
     <row r="202" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A202" t="str">
-        <f>CONCATENATE(C202," ",D202)</f>
+        <f t="shared" ref="A202:A233" si="7">CONCATENATE(C202," ",D202)</f>
         <v>Shuxin Tran</v>
       </c>
       <c r="B202" s="6" t="s">
@@ -8987,7 +8969,7 @@
     </row>
     <row r="203" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A203" t="str">
-        <f>CONCATENATE(C203," ",D203)</f>
+        <f t="shared" si="7"/>
         <v>Tony Tran</v>
       </c>
       <c r="B203" s="6" t="s">
@@ -9002,7 +8984,7 @@
     </row>
     <row r="204" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A204" t="str">
-        <f>CONCATENATE(C204," ",D204)</f>
+        <f t="shared" si="7"/>
         <v>Angelina Tostenson</v>
       </c>
       <c r="B204" s="6" t="s">
@@ -9017,7 +8999,7 @@
     </row>
     <row r="205" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A205" t="str">
-        <f>CONCATENATE(C205," ",D205)</f>
+        <f t="shared" si="7"/>
         <v>Osualdo Tom</v>
       </c>
       <c r="B205" s="6" t="s">
@@ -9032,7 +9014,7 @@
     </row>
     <row r="206" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A206" t="str">
-        <f>CONCATENATE(C206," ",D206)</f>
+        <f t="shared" si="7"/>
         <v>Cieara Zhou</v>
       </c>
       <c r="B206" s="6" t="s">
@@ -9047,7 +9029,7 @@
     </row>
     <row r="207" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A207" t="str">
-        <f>CONCATENATE(C207," ",D207)</f>
+        <f t="shared" si="7"/>
         <v>Aron Zhang</v>
       </c>
       <c r="B207" s="6" t="s">
@@ -9062,7 +9044,7 @@
     </row>
     <row r="208" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A208" t="str">
-        <f>CONCATENATE(C208," ",D208)</f>
+        <f t="shared" si="7"/>
         <v>Lennox Zhang</v>
       </c>
       <c r="B208" s="6" t="s">
@@ -9077,7 +9059,7 @@
     </row>
     <row r="209" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A209" t="str">
-        <f>CONCATENATE(C209," ",D209)</f>
+        <f t="shared" si="7"/>
         <v>William Zhang</v>
       </c>
       <c r="B209" s="6" t="s">
@@ -9092,7 +9074,7 @@
     </row>
     <row r="210" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A210" t="str">
-        <f>CONCATENATE(C210," ",D210)</f>
+        <f t="shared" si="7"/>
         <v>Frank Zhang</v>
       </c>
       <c r="B210" s="6" t="s">
@@ -9107,7 +9089,7 @@
     </row>
     <row r="211" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A211" t="str">
-        <f>CONCATENATE(C211," ",D211)</f>
+        <f t="shared" si="7"/>
         <v>Robert Zevallos</v>
       </c>
       <c r="B211" s="6" t="s">
@@ -9122,7 +9104,7 @@
     </row>
     <row r="212" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A212" t="str">
-        <f>CONCATENATE(C212," ",D212)</f>
+        <f t="shared" si="7"/>
         <v>Fritzgerald Zenner</v>
       </c>
       <c r="B212" s="6" t="s">
@@ -9137,7 +9119,7 @@
     </row>
     <row r="213" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A213" t="str">
-        <f>CONCATENATE(C213," ",D213)</f>
+        <f t="shared" si="7"/>
         <v>Nate Zeng</v>
       </c>
       <c r="B213" s="6" t="s">
@@ -9152,7 +9134,7 @@
     </row>
     <row r="214" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A214" t="str">
-        <f>CONCATENATE(C214," ",D214)</f>
+        <f t="shared" si="7"/>
         <v>Abel Zarza</v>
       </c>
       <c r="B214" s="6" t="s">
@@ -9167,7 +9149,7 @@
     </row>
     <row r="215" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A215" t="str">
-        <f>CONCATENATE(C215," ",D215)</f>
+        <f t="shared" si="7"/>
         <v>Juan Yu</v>
       </c>
       <c r="B215" s="6" t="s">
@@ -9182,7 +9164,7 @@
     </row>
     <row r="216" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A216" t="str">
-        <f>CONCATENATE(C216," ",D216)</f>
+        <f t="shared" si="7"/>
         <v>Emily Yu</v>
       </c>
       <c r="B216" s="6" t="s">
@@ -9197,7 +9179,7 @@
     </row>
     <row r="217" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A217" t="str">
-        <f>CONCATENATE(C217," ",D217)</f>
+        <f t="shared" si="7"/>
         <v>Kenny Yu</v>
       </c>
       <c r="B217" s="6" t="s">
@@ -9212,7 +9194,7 @@
     </row>
     <row r="218" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A218" t="str">
-        <f>CONCATENATE(C218," ",D218)</f>
+        <f t="shared" si="7"/>
         <v>Mimi Yip</v>
       </c>
       <c r="B218" s="6" t="s">
@@ -9227,7 +9209,7 @@
     </row>
     <row r="219" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A219" t="str">
-        <f>CONCATENATE(C219," ",D219)</f>
+        <f t="shared" si="7"/>
         <v>Emanuel Yi</v>
       </c>
       <c r="B219" s="6" t="s">
@@ -9242,7 +9224,7 @@
     </row>
     <row r="220" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A220" t="str">
-        <f>CONCATENATE(C220," ",D220)</f>
+        <f t="shared" si="7"/>
         <v>Gene Zlatev</v>
       </c>
       <c r="B220" s="6" t="s">
@@ -9257,7 +9239,7 @@
     </row>
     <row r="221" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A221" t="str">
-        <f>CONCATENATE(C221," ",D221)</f>
+        <f t="shared" si="7"/>
         <v>Bobbi Zinoman</v>
       </c>
       <c r="B221" s="6" t="s">
@@ -9272,7 +9254,7 @@
     </row>
     <row r="222" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A222" t="str">
-        <f>CONCATENATE(C222," ",D222)</f>
+        <f t="shared" si="7"/>
         <v>Griffen Zhu</v>
       </c>
       <c r="B222" s="6" t="s">
@@ -9287,7 +9269,7 @@
     </row>
     <row r="223" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A223" t="str">
-        <f>CONCATENATE(C223," ",D223)</f>
+        <f t="shared" si="7"/>
         <v>Connie Zhou</v>
       </c>
       <c r="B223" s="6" t="s">
@@ -9302,7 +9284,7 @@
     </row>
     <row r="224" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A224" t="str">
-        <f>CONCATENATE(C224," ",D224)</f>
+        <f t="shared" si="7"/>
         <v>Joshua Zhou</v>
       </c>
       <c r="B224" s="6" t="s">
@@ -9317,7 +9299,7 @@
     </row>
     <row r="225" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A225" t="str">
-        <f>CONCATENATE(C225," ",D225)</f>
+        <f t="shared" si="7"/>
         <v>Carissa Zhou</v>
       </c>
       <c r="B225" s="6" t="s">
@@ -9332,7 +9314,7 @@
     </row>
     <row r="226" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A226" t="str">
-        <f>CONCATENATE(C226," ",D226)</f>
+        <f t="shared" si="7"/>
         <v>Jorge Martinez</v>
       </c>
       <c r="B226" s="6" t="s">
@@ -9347,7 +9329,7 @@
     </row>
     <row r="227" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A227" t="str">
-        <f>CONCATENATE(C227," ",D227)</f>
+        <f t="shared" si="7"/>
         <v>Admiral Martinee</v>
       </c>
       <c r="B227" s="6" t="s">
@@ -9362,7 +9344,7 @@
     </row>
     <row r="228" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A228" t="str">
-        <f>CONCATENATE(C228," ",D228)</f>
+        <f t="shared" si="7"/>
         <v>Adam Martin</v>
       </c>
       <c r="B228" s="6" t="s">
@@ -9377,7 +9359,7 @@
     </row>
     <row r="229" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A229" t="str">
-        <f>CONCATENATE(C229," ",D229)</f>
+        <f t="shared" si="7"/>
         <v>Rilhiyah Mart</v>
       </c>
       <c r="B229" s="6" t="s">
@@ -9392,7 +9374,7 @@
     </row>
     <row r="230" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A230" t="str">
-        <f>CONCATENATE(C230," ",D230)</f>
+        <f t="shared" si="7"/>
         <v>Skylar Marrama</v>
       </c>
       <c r="B230" s="6" t="s">
@@ -9407,7 +9389,7 @@
     </row>
     <row r="231" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A231" t="str">
-        <f>CONCATENATE(C231," ",D231)</f>
+        <f t="shared" si="7"/>
         <v>Charlie Manalo</v>
       </c>
       <c r="B231" s="6" t="s">
@@ -9422,7 +9404,7 @@
     </row>
     <row r="232" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A232" t="str">
-        <f>CONCATENATE(C232," ",D232)</f>
+        <f t="shared" si="7"/>
         <v>Daniel Maddison</v>
       </c>
       <c r="B232" s="6" t="s">
@@ -9437,7 +9419,7 @@
     </row>
     <row r="233" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A233" t="str">
-        <f>CONCATENATE(C233," ",D233)</f>
+        <f t="shared" si="7"/>
         <v>Kayley Luu</v>
       </c>
       <c r="B233" s="6" t="s">
@@ -9452,7 +9434,7 @@
     </row>
     <row r="234" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A234" t="str">
-        <f>CONCATENATE(C234," ",D234)</f>
+        <f t="shared" ref="A234:A265" si="8">CONCATENATE(C234," ",D234)</f>
         <v>Laura Luna</v>
       </c>
       <c r="B234" s="6" t="s">
@@ -9467,7 +9449,7 @@
     </row>
     <row r="235" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A235" t="str">
-        <f>CONCATENATE(C235," ",D235)</f>
+        <f t="shared" si="8"/>
         <v>Kandace Lui</v>
       </c>
       <c r="B235" s="6" t="s">
@@ -9482,7 +9464,7 @@
     </row>
     <row r="236" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A236" t="str">
-        <f>CONCATENATE(C236," ",D236)</f>
+        <f t="shared" si="8"/>
         <v>Nuo Lou</v>
       </c>
       <c r="B236" s="6" t="s">
@@ -9497,7 +9479,7 @@
     </row>
     <row r="237" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A237" t="str">
-        <f>CONCATENATE(C237," ",D237)</f>
+        <f t="shared" si="8"/>
         <v>Walter Lopez</v>
       </c>
       <c r="B237" s="6" t="s">
@@ -9512,7 +9494,7 @@
     </row>
     <row r="238" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A238" t="str">
-        <f>CONCATENATE(C238," ",D238)</f>
+        <f t="shared" si="8"/>
         <v>Karoline Morgan</v>
       </c>
       <c r="B238" s="6" t="s">
@@ -9527,7 +9509,7 @@
     </row>
     <row r="239" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A239" t="str">
-        <f>CONCATENATE(C239," ",D239)</f>
+        <f t="shared" si="8"/>
         <v>Ketzia Moreno</v>
       </c>
       <c r="B239" s="6" t="s">
@@ -9542,7 +9524,7 @@
     </row>
     <row r="240" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A240" t="str">
-        <f>CONCATENATE(C240," ",D240)</f>
+        <f t="shared" si="8"/>
         <v>Aelafe Moore</v>
       </c>
       <c r="B240" s="6" t="s">
@@ -9557,7 +9539,7 @@
     </row>
     <row r="241" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A241" t="str">
-        <f>CONCATENATE(C241," ",D241)</f>
+        <f t="shared" si="8"/>
         <v>Janet Montevirgin</v>
       </c>
       <c r="B241" s="6" t="s">
@@ -9572,7 +9554,7 @@
     </row>
     <row r="242" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A242" t="str">
-        <f>CONCATENATE(C242," ",D242)</f>
+        <f t="shared" si="8"/>
         <v>Kenyon Mogilewski</v>
       </c>
       <c r="B242" s="6" t="s">
@@ -9587,7 +9569,7 @@
     </row>
     <row r="243" spans="1:4" ht="25.5" x14ac:dyDescent="0.55000000000000004">
       <c r="A243" t="str">
-        <f>CONCATENATE(C243," ",D243)</f>
+        <f t="shared" si="8"/>
         <v>Wangsen (Stanley) Mitchell</v>
       </c>
       <c r="B243" s="6" t="s">
@@ -9602,7 +9584,7 @@
     </row>
     <row r="244" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A244" t="str">
-        <f>CONCATENATE(C244," ",D244)</f>
+        <f t="shared" si="8"/>
         <v>Patrick Minsky</v>
       </c>
       <c r="B244" s="6" t="s">
@@ -9617,7 +9599,7 @@
     </row>
     <row r="245" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A245" t="str">
-        <f>CONCATENATE(C245," ",D245)</f>
+        <f t="shared" si="8"/>
         <v>Thane Mills</v>
       </c>
       <c r="B245" s="6" t="s">
@@ -9632,7 +9614,7 @@
     </row>
     <row r="246" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A246" t="str">
-        <f>CONCATENATE(C246," ",D246)</f>
+        <f t="shared" si="8"/>
         <v>Ryan Micael</v>
       </c>
       <c r="B246" s="6" t="s">
@@ -9647,7 +9629,7 @@
     </row>
     <row r="247" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A247" t="str">
-        <f>CONCATENATE(C247," ",D247)</f>
+        <f t="shared" si="8"/>
         <v>Ethan Merzenich</v>
       </c>
       <c r="B247" s="6" t="s">
@@ -9662,7 +9644,7 @@
     </row>
     <row r="248" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A248" t="str">
-        <f>CONCATENATE(C248," ",D248)</f>
+        <f t="shared" si="8"/>
         <v>Hana Merino</v>
       </c>
       <c r="B248" s="6" t="s">
@@ -9677,7 +9659,7 @@
     </row>
     <row r="249" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A249" t="str">
-        <f>CONCATENATE(C249," ",D249)</f>
+        <f t="shared" si="8"/>
         <v>Michelle Mendes</v>
       </c>
       <c r="B249" s="6" t="s">
@@ -9692,7 +9674,7 @@
     </row>
     <row r="250" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A250" t="str">
-        <f>CONCATENATE(C250," ",D250)</f>
+        <f t="shared" si="8"/>
         <v>Christian Mejia</v>
       </c>
       <c r="B250" s="6" t="s">
@@ -9707,7 +9689,7 @@
     </row>
     <row r="251" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A251" t="str">
-        <f>CONCATENATE(C251," ",D251)</f>
+        <f t="shared" si="8"/>
         <v>Jonathan Mei</v>
       </c>
       <c r="B251" s="6" t="s">
@@ -9722,7 +9704,7 @@
     </row>
     <row r="252" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A252" t="str">
-        <f>CONCATENATE(C252," ",D252)</f>
+        <f t="shared" si="8"/>
         <v>Cristiana McNary</v>
       </c>
       <c r="B252" s="6" t="s">
@@ -9737,7 +9719,7 @@
     </row>
     <row r="253" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A253" t="str">
-        <f>CONCATENATE(C253," ",D253)</f>
+        <f t="shared" si="8"/>
         <v>Tammy McLoughlin</v>
       </c>
       <c r="B253" s="6" t="s">
@@ -9752,7 +9734,7 @@
     </row>
     <row r="254" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A254" t="str">
-        <f>CONCATENATE(C254," ",D254)</f>
+        <f t="shared" si="8"/>
         <v>Amit McDonald</v>
       </c>
       <c r="B254" s="6" t="s">
@@ -9767,7 +9749,7 @@
     </row>
     <row r="255" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A255" t="str">
-        <f>CONCATENATE(C255," ",D255)</f>
+        <f t="shared" si="8"/>
         <v>Kailash McCaulley</v>
       </c>
       <c r="B255" s="6" t="s">
@@ -9782,7 +9764,7 @@
     </row>
     <row r="256" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A256" t="str">
-        <f>CONCATENATE(C256," ",D256)</f>
+        <f t="shared" si="8"/>
         <v>Winnie Maxwell</v>
       </c>
       <c r="B256" s="6" t="s">
@@ -9797,7 +9779,7 @@
     </row>
     <row r="257" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A257" t="str">
-        <f>CONCATENATE(C257," ",D257)</f>
+        <f t="shared" si="8"/>
         <v>Gaby Martinez</v>
       </c>
       <c r="B257" s="6" t="s">
@@ -9812,7 +9794,7 @@
     </row>
     <row r="258" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A258" t="str">
-        <f>CONCATENATE(C258," ",D258)</f>
+        <f t="shared" si="8"/>
         <v>Samuel Martinez</v>
       </c>
       <c r="B258" s="6" t="s">
@@ -9827,7 +9809,7 @@
     </row>
     <row r="259" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A259" t="str">
-        <f>CONCATENATE(C259," ",D259)</f>
+        <f t="shared" si="8"/>
         <v>Samuel Soephan</v>
       </c>
       <c r="B259" s="6" t="s">
@@ -9842,7 +9824,7 @@
     </row>
     <row r="260" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A260" t="str">
-        <f>CONCATENATE(C260," ",D260)</f>
+        <f t="shared" si="8"/>
         <v>Tom Smith</v>
       </c>
       <c r="B260" s="6" t="s">
@@ -9857,7 +9839,7 @@
     </row>
     <row r="261" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A261" t="str">
-        <f>CONCATENATE(C261," ",D261)</f>
+        <f t="shared" si="8"/>
         <v>Jake Smith</v>
       </c>
       <c r="B261" s="6" t="s">
@@ -9872,7 +9854,7 @@
     </row>
     <row r="262" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A262" t="str">
-        <f>CONCATENATE(C262," ",D262)</f>
+        <f t="shared" si="8"/>
         <v>Joseph Situ</v>
       </c>
       <c r="B262" s="6" t="s">
@@ -9887,7 +9869,7 @@
     </row>
     <row r="263" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A263" t="str">
-        <f>CONCATENATE(C263," ",D263)</f>
+        <f t="shared" si="8"/>
         <v>Jayshaun Singleton</v>
       </c>
       <c r="B263" s="6" t="s">
@@ -9902,7 +9884,7 @@
     </row>
     <row r="264" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A264" t="str">
-        <f>CONCATENATE(C264," ",D264)</f>
+        <f t="shared" si="8"/>
         <v>Branden Singh</v>
       </c>
       <c r="B264" s="6" t="s">
@@ -9917,7 +9899,7 @@
     </row>
     <row r="265" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A265" t="str">
-        <f>CONCATENATE(C265," ",D265)</f>
+        <f t="shared" si="8"/>
         <v>Elizabeth Singh</v>
       </c>
       <c r="B265" s="6" t="s">
@@ -9932,7 +9914,7 @@
     </row>
     <row r="266" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A266" t="str">
-        <f>CONCATENATE(C266," ",D266)</f>
+        <f t="shared" ref="A266:A297" si="9">CONCATENATE(C266," ",D266)</f>
         <v>Lamont Simmons</v>
       </c>
       <c r="B266" s="6" t="s">
@@ -9947,7 +9929,7 @@
     </row>
     <row r="267" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A267" t="str">
-        <f>CONCATENATE(C267," ",D267)</f>
+        <f t="shared" si="9"/>
         <v>Irvin Silverman</v>
       </c>
       <c r="B267" s="6" t="s">
@@ -9962,7 +9944,7 @@
     </row>
     <row r="268" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A268" t="str">
-        <f>CONCATENATE(C268," ",D268)</f>
+        <f t="shared" si="9"/>
         <v>Billy Shutt</v>
       </c>
       <c r="B268" s="6" t="s">
@@ -9977,7 +9959,7 @@
     </row>
     <row r="269" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A269" t="str">
-        <f>CONCATENATE(C269," ",D269)</f>
+        <f t="shared" si="9"/>
         <v>Lewis Shirozi</v>
       </c>
       <c r="B269" s="6" t="s">
@@ -9992,7 +9974,7 @@
     </row>
     <row r="270" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A270" t="str">
-        <f>CONCATENATE(C270," ",D270)</f>
+        <f t="shared" si="9"/>
         <v>Gilberto Shi</v>
       </c>
       <c r="B270" s="6" t="s">
@@ -10007,7 +9989,7 @@
     </row>
     <row r="271" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A271" t="str">
-        <f>CONCATENATE(C271," ",D271)</f>
+        <f t="shared" si="9"/>
         <v>Leila Shalf</v>
       </c>
       <c r="B271" s="6" t="s">
@@ -10022,7 +10004,7 @@
     </row>
     <row r="272" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A272" t="str">
-        <f>CONCATENATE(C272," ",D272)</f>
+        <f t="shared" si="9"/>
         <v>Andrea Servin</v>
       </c>
       <c r="B272" s="6" t="s">
@@ -10037,7 +10019,7 @@
     </row>
     <row r="273" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A273" t="str">
-        <f>CONCATENATE(C273," ",D273)</f>
+        <f t="shared" si="9"/>
         <v>Raymond Schooling</v>
       </c>
       <c r="B273" s="6" t="s">
@@ -10052,7 +10034,7 @@
     </row>
     <row r="274" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A274" t="str">
-        <f>CONCATENATE(C274," ",D274)</f>
+        <f t="shared" si="9"/>
         <v>Tony Schniedergers</v>
       </c>
       <c r="B274" s="6" t="s">
@@ -10067,7 +10049,7 @@
     </row>
     <row r="275" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A275" t="str">
-        <f>CONCATENATE(C275," ",D275)</f>
+        <f t="shared" si="9"/>
         <v>Macie Schneidinger</v>
       </c>
       <c r="B275" s="6" t="s">
@@ -10082,7 +10064,7 @@
     </row>
     <row r="276" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A276" t="str">
-        <f>CONCATENATE(C276," ",D276)</f>
+        <f t="shared" si="9"/>
         <v>Jair Saucedo</v>
       </c>
       <c r="B276" s="6" t="s">
@@ -10097,7 +10079,7 @@
     </row>
     <row r="277" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A277" t="str">
-        <f>CONCATENATE(C277," ",D277)</f>
+        <f t="shared" si="9"/>
         <v>Tristan Santana</v>
       </c>
       <c r="B277" s="6" t="s">
@@ -10112,7 +10094,7 @@
     </row>
     <row r="278" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A278" t="str">
-        <f>CONCATENATE(C278," ",D278)</f>
+        <f t="shared" si="9"/>
         <v>Gavin Orla-Bukowski</v>
       </c>
       <c r="B278" s="6" t="s">
@@ -10127,7 +10109,7 @@
     </row>
     <row r="279" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A279" t="str">
-        <f>CONCATENATE(C279," ",D279)</f>
+        <f t="shared" si="9"/>
         <v>Minnie Ong</v>
       </c>
       <c r="B279" s="6" t="s">
@@ -10142,7 +10124,7 @@
     </row>
     <row r="280" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A280" t="str">
-        <f>CONCATENATE(C280," ",D280)</f>
+        <f t="shared" si="9"/>
         <v>Andy Olson</v>
       </c>
       <c r="B280" s="6" t="s">
@@ -10157,7 +10139,7 @@
     </row>
     <row r="281" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A281" t="str">
-        <f>CONCATENATE(C281," ",D281)</f>
+        <f t="shared" si="9"/>
         <v>Quiante Olosiman</v>
       </c>
       <c r="B281" s="6" t="s">
@@ -10172,11 +10154,11 @@
     </row>
     <row r="282" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A282" t="str">
-        <f>CONCATENATE(C282," ",D282)</f>
+        <f t="shared" si="9"/>
         <v>Raymond Oddone</v>
       </c>
       <c r="B282" s="6" t="s">
-        <v>917</v>
+        <v>911</v>
       </c>
       <c r="C282" s="6" t="s">
         <v>443</v>
@@ -10187,11 +10169,11 @@
     </row>
     <row r="283" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A283" t="str">
-        <f>CONCATENATE(C283," ",D283)</f>
+        <f t="shared" si="9"/>
         <v>Alex Norbu</v>
       </c>
       <c r="B283" s="6" t="s">
-        <v>917</v>
+        <v>911</v>
       </c>
       <c r="C283" s="6" t="s">
         <v>237</v>
@@ -10202,11 +10184,11 @@
     </row>
     <row r="284" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A284" t="str">
-        <f>CONCATENATE(C284," ",D284)</f>
+        <f t="shared" si="9"/>
         <v>Carlos Nieves</v>
       </c>
       <c r="B284" s="6" t="s">
-        <v>917</v>
+        <v>911</v>
       </c>
       <c r="C284" s="6" t="s">
         <v>247</v>
@@ -10217,11 +10199,11 @@
     </row>
     <row r="285" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A285" t="str">
-        <f>CONCATENATE(C285," ",D285)</f>
+        <f t="shared" si="9"/>
         <v>David Nguyen</v>
       </c>
       <c r="B285" s="6" t="s">
-        <v>917</v>
+        <v>911</v>
       </c>
       <c r="C285" s="6" t="s">
         <v>205</v>
@@ -10232,11 +10214,11 @@
     </row>
     <row r="286" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A286" t="str">
-        <f>CONCATENATE(C286," ",D286)</f>
+        <f t="shared" si="9"/>
         <v>JingJun Nguyen</v>
       </c>
       <c r="B286" s="6" t="s">
-        <v>917</v>
+        <v>911</v>
       </c>
       <c r="C286" s="6" t="s">
         <v>396</v>
@@ -10247,11 +10229,11 @@
     </row>
     <row r="287" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A287" t="str">
-        <f>CONCATENATE(C287," ",D287)</f>
+        <f t="shared" si="9"/>
         <v>Joshua Nguyen</v>
       </c>
       <c r="B287" s="6" t="s">
-        <v>917</v>
+        <v>911</v>
       </c>
       <c r="C287" s="6" t="s">
         <v>34</v>
@@ -10262,11 +10244,11 @@
     </row>
     <row r="288" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A288" t="str">
-        <f>CONCATENATE(C288," ",D288)</f>
+        <f t="shared" si="9"/>
         <v>Kai Nguyen</v>
       </c>
       <c r="B288" s="6" t="s">
-        <v>917</v>
+        <v>911</v>
       </c>
       <c r="C288" s="6" t="s">
         <v>447</v>
@@ -10277,11 +10259,11 @@
     </row>
     <row r="289" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A289" t="str">
-        <f>CONCATENATE(C289," ",D289)</f>
+        <f t="shared" si="9"/>
         <v>Sydney Nguyen</v>
       </c>
       <c r="B289" s="6" t="s">
-        <v>917</v>
+        <v>911</v>
       </c>
       <c r="C289" s="6" t="s">
         <v>330</v>
@@ -10292,7 +10274,7 @@
     </row>
     <row r="290" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A290" t="str">
-        <f>CONCATENATE(C290," ",D290)</f>
+        <f t="shared" si="9"/>
         <v>Agustin Lopez</v>
       </c>
       <c r="B290" s="6" t="s">
@@ -10307,7 +10289,7 @@
     </row>
     <row r="291" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A291" t="str">
-        <f>CONCATENATE(C291," ",D291)</f>
+        <f t="shared" si="9"/>
         <v>Luis Lopez</v>
       </c>
       <c r="B291" s="6" t="s">
@@ -10322,7 +10304,7 @@
     </row>
     <row r="292" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A292" t="str">
-        <f>CONCATENATE(C292," ",D292)</f>
+        <f t="shared" si="9"/>
         <v>Huabin Lodoe</v>
       </c>
       <c r="B292" s="6" t="s">
@@ -10337,7 +10319,7 @@
     </row>
     <row r="293" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A293" t="str">
-        <f>CONCATENATE(C293," ",D293)</f>
+        <f t="shared" si="9"/>
         <v>Hien Liu</v>
       </c>
       <c r="B293" s="6" t="s">
@@ -10352,7 +10334,7 @@
     </row>
     <row r="294" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A294" t="str">
-        <f>CONCATENATE(C294," ",D294)</f>
+        <f t="shared" si="9"/>
         <v>Donovan Lira</v>
       </c>
       <c r="B294" s="6" t="s">
@@ -10367,7 +10349,7 @@
     </row>
     <row r="295" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A295" t="str">
-        <f>CONCATENATE(C295," ",D295)</f>
+        <f t="shared" si="9"/>
         <v>Alex Lintao</v>
       </c>
       <c r="B295" s="6" t="s">
@@ -10382,7 +10364,7 @@
     </row>
     <row r="296" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A296" t="str">
-        <f>CONCATENATE(C296," ",D296)</f>
+        <f t="shared" si="9"/>
         <v>Jiani Ligutan</v>
       </c>
       <c r="B296" s="6" t="s">
@@ -10397,7 +10379,7 @@
     </row>
     <row r="297" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A297" t="str">
-        <f>CONCATENATE(C297," ",D297)</f>
+        <f t="shared" si="9"/>
         <v>Michael Liang</v>
       </c>
       <c r="B297" s="6" t="s">
@@ -10412,7 +10394,7 @@
     </row>
     <row r="298" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A298" t="str">
-        <f>CONCATENATE(C298," ",D298)</f>
+        <f t="shared" ref="A298:A316" si="10">CONCATENATE(C298," ",D298)</f>
         <v>Jeanie Li</v>
       </c>
       <c r="B298" s="6" t="s">
@@ -10427,7 +10409,7 @@
     </row>
     <row r="299" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A299" t="str">
-        <f>CONCATENATE(C299," ",D299)</f>
+        <f t="shared" si="10"/>
         <v>Carvell Levi</v>
       </c>
       <c r="B299" s="6" t="s">
@@ -10442,7 +10424,7 @@
     </row>
     <row r="300" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A300" t="str">
-        <f>CONCATENATE(C300," ",D300)</f>
+        <f t="shared" si="10"/>
         <v>Calvin Leung</v>
       </c>
       <c r="B300" s="6" t="s">
@@ -10457,7 +10439,7 @@
     </row>
     <row r="301" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A301" t="str">
-        <f>CONCATENATE(C301," ",D301)</f>
+        <f t="shared" si="10"/>
         <v>Kai Quale</v>
       </c>
       <c r="B301" s="6" t="s">
@@ -10472,7 +10454,7 @@
     </row>
     <row r="302" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A302" t="str">
-        <f>CONCATENATE(C302," ",D302)</f>
+        <f t="shared" si="10"/>
         <v>Maya Qiu</v>
       </c>
       <c r="B302" s="6" t="s">
@@ -10487,7 +10469,7 @@
     </row>
     <row r="303" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A303" t="str">
-        <f>CONCATENATE(C303," ",D303)</f>
+        <f t="shared" si="10"/>
         <v>Alex Priesto</v>
       </c>
       <c r="B303" s="6" t="s">
@@ -10502,7 +10484,7 @@
     </row>
     <row r="304" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A304" t="str">
-        <f>CONCATENATE(C304," ",D304)</f>
+        <f t="shared" si="10"/>
         <v>Cole Prendergast</v>
       </c>
       <c r="B304" s="6" t="s">
@@ -10517,7 +10499,7 @@
     </row>
     <row r="305" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A305" t="str">
-        <f>CONCATENATE(C305," ",D305)</f>
+        <f t="shared" si="10"/>
         <v>Junior Pratt</v>
       </c>
       <c r="B305" s="6" t="s">
@@ -10532,7 +10514,7 @@
     </row>
     <row r="306" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A306" t="str">
-        <f>CONCATENATE(C306," ",D306)</f>
+        <f t="shared" si="10"/>
         <v>Simranjit Poveda</v>
       </c>
       <c r="B306" s="6" t="s">
@@ -10547,7 +10529,7 @@
     </row>
     <row r="307" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A307" t="str">
-        <f>CONCATENATE(C307," ",D307)</f>
+        <f t="shared" si="10"/>
         <v>Daniela Portillo</v>
       </c>
       <c r="B307" s="6" t="s">
@@ -10562,7 +10544,7 @@
     </row>
     <row r="308" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A308" t="str">
-        <f>CONCATENATE(C308," ",D308)</f>
+        <f t="shared" si="10"/>
         <v>Athorva Pietropooli</v>
       </c>
       <c r="B308" s="6" t="s">
@@ -10577,7 +10559,7 @@
     </row>
     <row r="309" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A309" t="str">
-        <f>CONCATENATE(C309," ",D309)</f>
+        <f t="shared" si="10"/>
         <v>Kelsey Pierce</v>
       </c>
       <c r="B309" s="6" t="s">
@@ -10592,7 +10574,7 @@
     </row>
     <row r="310" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A310" t="str">
-        <f>CONCATENATE(C310," ",D310)</f>
+        <f t="shared" si="10"/>
         <v>William Piccillo</v>
       </c>
       <c r="B310" s="6" t="s">
@@ -10607,7 +10589,7 @@
     </row>
     <row r="311" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A311" t="str">
-        <f>CONCATENATE(C311," ",D311)</f>
+        <f t="shared" si="10"/>
         <v>Sara Phung</v>
       </c>
       <c r="B311" s="6" t="s">
@@ -10622,7 +10604,7 @@
     </row>
     <row r="312" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A312" t="str">
-        <f>CONCATENATE(C312," ",D312)</f>
+        <f t="shared" si="10"/>
         <v>Angelina Phoumivong</v>
       </c>
       <c r="B312" s="6" t="s">
@@ -10637,7 +10619,7 @@
     </row>
     <row r="313" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A313" t="str">
-        <f>CONCATENATE(C313," ",D313)</f>
+        <f t="shared" si="10"/>
         <v>Christian Pereda</v>
       </c>
       <c r="B313" s="6" t="s">
@@ -10652,7 +10634,7 @@
     </row>
     <row r="314" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A314" t="str">
-        <f>CONCATENATE(C314," ",D314)</f>
+        <f t="shared" si="10"/>
         <v>Gabriel Peng</v>
       </c>
       <c r="B314" s="6" t="s">
@@ -10667,7 +10649,7 @@
     </row>
     <row r="315" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A315" t="str">
-        <f>CONCATENATE(C315," ",D315)</f>
+        <f t="shared" si="10"/>
         <v>Sarbjot Pedersen</v>
       </c>
       <c r="B315" s="6" t="s">
@@ -10682,7 +10664,7 @@
     </row>
     <row r="316" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A316" t="str">
-        <f>CONCATENATE(C316," ",D316)</f>
+        <f t="shared" si="10"/>
         <v>Tiffany Pareja</v>
       </c>
       <c r="B316" s="6" t="s">
@@ -10727,8 +10709,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B24"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A12" sqref="A12"/>
+    <sheetView tabSelected="1" topLeftCell="A6" workbookViewId="0">
+      <selection activeCell="A25" sqref="A25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.89453125" defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
@@ -10819,7 +10801,7 @@
     </row>
     <row r="11" spans="1:2" ht="18.899999999999999" customHeight="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A11" s="6" t="s">
-        <v>808</v>
+        <v>793</v>
       </c>
       <c r="B11">
         <v>250</v>
@@ -10975,7 +10957,7 @@
       </c>
       <c r="C2">
         <f t="shared" ref="C2:C36" ca="1" si="0">RANDBETWEEN(1,100)</f>
-        <v>31</v>
+        <v>84</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.55000000000000004">
@@ -10987,7 +10969,7 @@
       </c>
       <c r="C3">
         <f t="shared" ca="1" si="0"/>
-        <v>20</v>
+        <v>26</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.55000000000000004">
@@ -10999,7 +10981,7 @@
       </c>
       <c r="C4">
         <f t="shared" ca="1" si="0"/>
-        <v>19</v>
+        <v>8</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.55000000000000004">
@@ -11011,7 +10993,7 @@
       </c>
       <c r="C5">
         <f t="shared" ca="1" si="0"/>
-        <v>49</v>
+        <v>64</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.55000000000000004">
@@ -11023,7 +11005,7 @@
       </c>
       <c r="C6">
         <f t="shared" ca="1" si="0"/>
-        <v>95</v>
+        <v>75</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.55000000000000004">
@@ -11035,7 +11017,7 @@
       </c>
       <c r="C7">
         <f t="shared" ca="1" si="0"/>
-        <v>64</v>
+        <v>58</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.55000000000000004">
@@ -11047,7 +11029,7 @@
       </c>
       <c r="C8">
         <f t="shared" ca="1" si="0"/>
-        <v>18</v>
+        <v>71</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.55000000000000004">
@@ -11059,7 +11041,7 @@
       </c>
       <c r="C9">
         <f t="shared" ca="1" si="0"/>
-        <v>40</v>
+        <v>72</v>
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.55000000000000004">
@@ -11071,7 +11053,7 @@
       </c>
       <c r="C10">
         <f t="shared" ca="1" si="0"/>
-        <v>76</v>
+        <v>49</v>
       </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.55000000000000004">
@@ -11083,7 +11065,7 @@
       </c>
       <c r="C11">
         <f t="shared" ca="1" si="0"/>
-        <v>72</v>
+        <v>43</v>
       </c>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.55000000000000004">
@@ -11095,7 +11077,7 @@
       </c>
       <c r="C12">
         <f t="shared" ca="1" si="0"/>
-        <v>64</v>
+        <v>86</v>
       </c>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.55000000000000004">
@@ -11107,7 +11089,7 @@
       </c>
       <c r="C13">
         <f t="shared" ca="1" si="0"/>
-        <v>13</v>
+        <v>93</v>
       </c>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.55000000000000004">
@@ -11130,7 +11112,7 @@
       </c>
       <c r="C15">
         <f t="shared" ca="1" si="0"/>
-        <v>56</v>
+        <v>60</v>
       </c>
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.55000000000000004">
@@ -11142,7 +11124,7 @@
       </c>
       <c r="C16">
         <f t="shared" ca="1" si="0"/>
-        <v>51</v>
+        <v>82</v>
       </c>
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.55000000000000004">
@@ -11154,7 +11136,7 @@
       </c>
       <c r="C17">
         <f t="shared" ca="1" si="0"/>
-        <v>54</v>
+        <v>76</v>
       </c>
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.55000000000000004">
@@ -11166,7 +11148,7 @@
       </c>
       <c r="C18">
         <f t="shared" ca="1" si="0"/>
-        <v>63</v>
+        <v>43</v>
       </c>
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.55000000000000004">
@@ -11178,7 +11160,7 @@
       </c>
       <c r="C19">
         <f t="shared" ca="1" si="0"/>
-        <v>78</v>
+        <v>72</v>
       </c>
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.55000000000000004">
@@ -11190,7 +11172,7 @@
       </c>
       <c r="C20">
         <f t="shared" ca="1" si="0"/>
-        <v>51</v>
+        <v>47</v>
       </c>
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.55000000000000004">
@@ -11202,7 +11184,7 @@
       </c>
       <c r="C21">
         <f t="shared" ca="1" si="0"/>
-        <v>19</v>
+        <v>66</v>
       </c>
     </row>
     <row r="22" spans="1:3" x14ac:dyDescent="0.55000000000000004">
@@ -11214,7 +11196,7 @@
       </c>
       <c r="C22">
         <f t="shared" ca="1" si="0"/>
-        <v>88</v>
+        <v>42</v>
       </c>
     </row>
     <row r="23" spans="1:3" x14ac:dyDescent="0.55000000000000004">
@@ -11226,7 +11208,7 @@
       </c>
       <c r="C23">
         <f t="shared" ca="1" si="0"/>
-        <v>22</v>
+        <v>64</v>
       </c>
     </row>
     <row r="24" spans="1:3" x14ac:dyDescent="0.55000000000000004">
@@ -11238,7 +11220,7 @@
       </c>
       <c r="C24">
         <f t="shared" ca="1" si="0"/>
-        <v>62</v>
+        <v>25</v>
       </c>
     </row>
     <row r="25" spans="1:3" x14ac:dyDescent="0.55000000000000004">
@@ -11261,7 +11243,7 @@
       </c>
       <c r="C26">
         <f t="shared" ca="1" si="0"/>
-        <v>86</v>
+        <v>81</v>
       </c>
     </row>
     <row r="27" spans="1:3" x14ac:dyDescent="0.55000000000000004">
@@ -11273,7 +11255,7 @@
       </c>
       <c r="C27">
         <f t="shared" ca="1" si="0"/>
-        <v>96</v>
+        <v>67</v>
       </c>
     </row>
     <row r="28" spans="1:3" x14ac:dyDescent="0.55000000000000004">
@@ -11285,7 +11267,7 @@
       </c>
       <c r="C28">
         <f t="shared" ca="1" si="0"/>
-        <v>82</v>
+        <v>26</v>
       </c>
     </row>
     <row r="29" spans="1:3" x14ac:dyDescent="0.55000000000000004">
@@ -11297,7 +11279,7 @@
       </c>
       <c r="C29">
         <f t="shared" ca="1" si="0"/>
-        <v>62</v>
+        <v>95</v>
       </c>
     </row>
     <row r="30" spans="1:3" x14ac:dyDescent="0.55000000000000004">
@@ -11320,7 +11302,7 @@
       </c>
       <c r="C31">
         <f t="shared" ca="1" si="0"/>
-        <v>13</v>
+        <v>100</v>
       </c>
     </row>
     <row r="32" spans="1:3" x14ac:dyDescent="0.55000000000000004">
@@ -11332,7 +11314,7 @@
       </c>
       <c r="C32">
         <f t="shared" ca="1" si="0"/>
-        <v>28</v>
+        <v>16</v>
       </c>
     </row>
     <row r="33" spans="1:3" x14ac:dyDescent="0.55000000000000004">
@@ -11344,7 +11326,7 @@
       </c>
       <c r="C33">
         <f t="shared" ca="1" si="0"/>
-        <v>5</v>
+        <v>36</v>
       </c>
     </row>
     <row r="34" spans="1:3" x14ac:dyDescent="0.55000000000000004">
@@ -11356,7 +11338,7 @@
       </c>
       <c r="C34">
         <f t="shared" ca="1" si="0"/>
-        <v>95</v>
+        <v>70</v>
       </c>
     </row>
     <row r="35" spans="1:3" x14ac:dyDescent="0.55000000000000004">
@@ -11368,7 +11350,7 @@
       </c>
       <c r="C35">
         <f t="shared" ca="1" si="0"/>
-        <v>95</v>
+        <v>61</v>
       </c>
     </row>
     <row r="36" spans="1:3" x14ac:dyDescent="0.55000000000000004">
@@ -11380,7 +11362,7 @@
       </c>
       <c r="C36">
         <f t="shared" ca="1" si="0"/>
-        <v>29</v>
+        <v>46</v>
       </c>
     </row>
     <row r="37" spans="1:3" x14ac:dyDescent="0.55000000000000004">
@@ -11403,7 +11385,7 @@
       </c>
       <c r="C38">
         <f t="shared" ref="C38:C56" ca="1" si="1">RANDBETWEEN(1,100)</f>
-        <v>36</v>
+        <v>10</v>
       </c>
     </row>
     <row r="39" spans="1:3" x14ac:dyDescent="0.55000000000000004">
@@ -11415,7 +11397,7 @@
       </c>
       <c r="C39">
         <f t="shared" ca="1" si="1"/>
-        <v>33</v>
+        <v>78</v>
       </c>
     </row>
     <row r="40" spans="1:3" x14ac:dyDescent="0.55000000000000004">
@@ -11427,7 +11409,7 @@
       </c>
       <c r="C40">
         <f t="shared" ca="1" si="1"/>
-        <v>85</v>
+        <v>7</v>
       </c>
     </row>
     <row r="41" spans="1:3" x14ac:dyDescent="0.55000000000000004">
@@ -11439,7 +11421,7 @@
       </c>
       <c r="C41">
         <f t="shared" ca="1" si="1"/>
-        <v>61</v>
+        <v>85</v>
       </c>
     </row>
     <row r="42" spans="1:3" x14ac:dyDescent="0.55000000000000004">
@@ -11451,7 +11433,7 @@
       </c>
       <c r="C42">
         <f t="shared" ca="1" si="1"/>
-        <v>88</v>
+        <v>33</v>
       </c>
     </row>
     <row r="43" spans="1:3" x14ac:dyDescent="0.55000000000000004">
@@ -11463,7 +11445,7 @@
       </c>
       <c r="C43">
         <f t="shared" ca="1" si="1"/>
-        <v>80</v>
+        <v>33</v>
       </c>
     </row>
     <row r="44" spans="1:3" x14ac:dyDescent="0.55000000000000004">
@@ -11475,7 +11457,7 @@
       </c>
       <c r="C44">
         <f t="shared" ca="1" si="1"/>
-        <v>30</v>
+        <v>22</v>
       </c>
     </row>
     <row r="45" spans="1:3" x14ac:dyDescent="0.55000000000000004">
@@ -11498,7 +11480,7 @@
       </c>
       <c r="C46">
         <f t="shared" ca="1" si="1"/>
-        <v>26</v>
+        <v>43</v>
       </c>
     </row>
     <row r="47" spans="1:3" x14ac:dyDescent="0.55000000000000004">
@@ -11510,7 +11492,7 @@
       </c>
       <c r="C47">
         <f t="shared" ca="1" si="1"/>
-        <v>47</v>
+        <v>41</v>
       </c>
     </row>
     <row r="48" spans="1:3" x14ac:dyDescent="0.55000000000000004">
@@ -11522,7 +11504,7 @@
       </c>
       <c r="C48">
         <f t="shared" ca="1" si="1"/>
-        <v>1</v>
+        <v>64</v>
       </c>
     </row>
     <row r="49" spans="1:3" x14ac:dyDescent="0.55000000000000004">
@@ -11534,7 +11516,7 @@
       </c>
       <c r="C49">
         <f t="shared" ca="1" si="1"/>
-        <v>51</v>
+        <v>27</v>
       </c>
     </row>
     <row r="50" spans="1:3" x14ac:dyDescent="0.55000000000000004">
@@ -11557,7 +11539,7 @@
       </c>
       <c r="C51">
         <f t="shared" ca="1" si="1"/>
-        <v>35</v>
+        <v>76</v>
       </c>
     </row>
     <row r="52" spans="1:3" x14ac:dyDescent="0.55000000000000004">
@@ -11569,7 +11551,7 @@
       </c>
       <c r="C52">
         <f t="shared" ca="1" si="1"/>
-        <v>25</v>
+        <v>45</v>
       </c>
     </row>
     <row r="53" spans="1:3" x14ac:dyDescent="0.55000000000000004">
@@ -11581,7 +11563,7 @@
       </c>
       <c r="C53">
         <f t="shared" ca="1" si="1"/>
-        <v>91</v>
+        <v>79</v>
       </c>
     </row>
     <row r="54" spans="1:3" x14ac:dyDescent="0.55000000000000004">
@@ -11593,7 +11575,7 @@
       </c>
       <c r="C54">
         <f t="shared" ca="1" si="1"/>
-        <v>94</v>
+        <v>79</v>
       </c>
     </row>
     <row r="55" spans="1:3" x14ac:dyDescent="0.55000000000000004">
@@ -11605,7 +11587,7 @@
       </c>
       <c r="C55">
         <f t="shared" ca="1" si="1"/>
-        <v>82</v>
+        <v>95</v>
       </c>
     </row>
     <row r="56" spans="1:3" x14ac:dyDescent="0.55000000000000004">
@@ -11617,7 +11599,7 @@
       </c>
       <c r="C56">
         <f t="shared" ca="1" si="1"/>
-        <v>75</v>
+        <v>90</v>
       </c>
     </row>
     <row r="57" spans="1:3" x14ac:dyDescent="0.55000000000000004">

</xml_diff>